<commit_message>
2022 PAV player updates and round 18 2022 predictions and data updates
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Brisbane_stats.xlsx
+++ b/django_AFL_ML/Data/Brisbane_stats.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IT102"/>
+  <dimension ref="A1:IZ102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="HZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="IL36" activeCellId="0" sqref="IL36"/>
@@ -1222,8 +1222,26 @@
       <c r="IS1" s="2" t="n">
         <v>10621</v>
       </c>
-      <c r="IT1" t="n">
+      <c r="IT1" s="2" t="n">
         <v>10628</v>
+      </c>
+      <c r="IU1" s="2" t="n">
+        <v>10634</v>
+      </c>
+      <c r="IV1" s="2" t="n">
+        <v>10648</v>
+      </c>
+      <c r="IW1" s="2" t="n">
+        <v>10649</v>
+      </c>
+      <c r="IX1" s="2" t="n">
+        <v>10664</v>
+      </c>
+      <c r="IY1" s="2" t="n">
+        <v>10670</v>
+      </c>
+      <c r="IZ1" t="n">
+        <v>10679</v>
       </c>
     </row>
     <row r="2" ht="13.9" customHeight="1" s="3">
@@ -1988,7 +2006,25 @@
       <c r="IS2" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="IT2" t="n">
+      <c r="IT2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IU2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IV2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IW2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IX2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IY2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IZ2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2754,8 +2790,26 @@
       <c r="IS3" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="IT3" t="n">
+      <c r="IT3" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="IU3" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IV3" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="IW3" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="IX3" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="IY3" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="IZ3" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="4" ht="13.9" customHeight="1" s="3">
@@ -3520,8 +3574,26 @@
       <c r="IS4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IT4" t="n">
+      <c r="IT4" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="IU4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IV4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IW4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IX4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IY4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IZ4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="13.9" customHeight="1" s="3">
@@ -4286,8 +4358,26 @@
       <c r="IS5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IT5" t="n">
+      <c r="IT5" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="IU5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IV5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IW5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IX5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IY5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IZ5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="13.9" customHeight="1" s="3">
@@ -5052,8 +5142,26 @@
       <c r="IS6" s="2" t="n">
         <v>102</v>
       </c>
-      <c r="IT6" t="n">
+      <c r="IT6" s="2" t="n">
         <v>112</v>
+      </c>
+      <c r="IU6" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="IV6" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="IW6" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="IX6" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="IY6" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="IZ6" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="7" ht="13.9" customHeight="1" s="3">
@@ -5818,8 +5926,26 @@
       <c r="IS7" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="IT7" t="n">
+      <c r="IT7" s="2" t="n">
         <v>117</v>
+      </c>
+      <c r="IU7" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="IV7" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="IW7" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="IX7" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="IY7" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="IZ7" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="8" ht="13.9" customHeight="1" s="3">
@@ -6584,8 +6710,26 @@
       <c r="IS8" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="IT8" t="n">
+      <c r="IT8" s="2" t="n">
         <v>-5</v>
+      </c>
+      <c r="IU8" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="IV8" s="2" t="n">
+        <v>-14</v>
+      </c>
+      <c r="IW8" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="IX8" s="2" t="n">
+        <v>-64</v>
+      </c>
+      <c r="IY8" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="IZ8" t="n">
+        <v>-10</v>
       </c>
     </row>
     <row r="9" ht="13.9" customHeight="1" s="3">
@@ -7350,7 +7494,25 @@
       <c r="IS9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IT9" t="n">
+      <c r="IT9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IU9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IV9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IW9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IX9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="IY9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IZ9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8116,8 +8278,26 @@
       <c r="IS10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IT10" t="n">
+      <c r="IT10" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="IU10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IV10" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IW10" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="IX10" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IY10" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="IZ10" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="11" ht="13.9" customHeight="1" s="3">
@@ -8882,8 +9062,26 @@
       <c r="IS11" s="2" t="n">
         <v>224</v>
       </c>
-      <c r="IT11" t="n">
+      <c r="IT11" s="2" t="n">
         <v>225</v>
+      </c>
+      <c r="IU11" s="2" t="n">
+        <v>215</v>
+      </c>
+      <c r="IV11" s="2" t="n">
+        <v>227</v>
+      </c>
+      <c r="IW11" s="2" t="n">
+        <v>253</v>
+      </c>
+      <c r="IX11" s="2" t="n">
+        <v>211</v>
+      </c>
+      <c r="IY11" s="2" t="n">
+        <v>243</v>
+      </c>
+      <c r="IZ11" t="n">
+        <v>195</v>
       </c>
     </row>
     <row r="12" ht="13.9" customHeight="1" s="3">
@@ -9648,8 +9846,26 @@
       <c r="IS12" s="2" t="n">
         <v>119</v>
       </c>
-      <c r="IT12" t="n">
+      <c r="IT12" s="2" t="n">
         <v>124</v>
+      </c>
+      <c r="IU12" s="2" t="n">
+        <v>148</v>
+      </c>
+      <c r="IV12" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="IW12" s="2" t="n">
+        <v>115</v>
+      </c>
+      <c r="IX12" s="2" t="n">
+        <v>121</v>
+      </c>
+      <c r="IY12" s="2" t="n">
+        <v>101</v>
+      </c>
+      <c r="IZ12" t="n">
+        <v>106</v>
       </c>
     </row>
     <row r="13" ht="13.9" customHeight="1" s="3">
@@ -10414,8 +10630,26 @@
       <c r="IS13" s="2" t="n">
         <v>343</v>
       </c>
-      <c r="IT13" t="n">
+      <c r="IT13" s="2" t="n">
         <v>349</v>
+      </c>
+      <c r="IU13" s="2" t="n">
+        <v>363</v>
+      </c>
+      <c r="IV13" s="2" t="n">
+        <v>355</v>
+      </c>
+      <c r="IW13" s="2" t="n">
+        <v>368</v>
+      </c>
+      <c r="IX13" s="2" t="n">
+        <v>332</v>
+      </c>
+      <c r="IY13" s="2" t="n">
+        <v>344</v>
+      </c>
+      <c r="IZ13" t="n">
+        <v>301</v>
       </c>
     </row>
     <row r="14" ht="13.9" customHeight="1" s="3">
@@ -11180,8 +11414,26 @@
       <c r="IS14" s="2" t="n">
         <v>1.88</v>
       </c>
-      <c r="IT14" t="n">
+      <c r="IT14" s="2" t="n">
         <v>1.81</v>
+      </c>
+      <c r="IU14" s="2" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="IV14" s="2" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="IW14" s="2" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="IX14" s="2" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="IY14" s="2" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="IZ14" t="n">
+        <v>1.84</v>
       </c>
     </row>
     <row r="15" ht="13.9" customHeight="1" s="3">
@@ -11946,8 +12198,26 @@
       <c r="IS15" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="IT15" t="n">
+      <c r="IT15" s="2" t="n">
         <v>84</v>
+      </c>
+      <c r="IU15" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="IV15" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="IW15" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="IX15" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="IY15" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="IZ15" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="16" ht="13.9" customHeight="1" s="3">
@@ -12712,8 +12982,26 @@
       <c r="IS16" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="IT16" t="n">
+      <c r="IT16" s="2" t="n">
         <v>63</v>
+      </c>
+      <c r="IU16" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="IV16" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="IW16" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="IX16" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="IY16" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="IZ16" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="17" ht="13.9" customHeight="1" s="3">
@@ -13478,8 +13766,26 @@
       <c r="IS17" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="IT17" t="n">
+      <c r="IT17" s="2" t="n">
         <v>71</v>
+      </c>
+      <c r="IU17" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="IV17" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="IW17" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="IX17" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="IY17" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="IZ17" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="18" ht="13.9" customHeight="1" s="3">
@@ -14244,8 +14550,26 @@
       <c r="IS18" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="IT18" t="n">
+      <c r="IT18" s="2" t="n">
         <v>27</v>
+      </c>
+      <c r="IU18" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="IV18" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="IW18" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="IX18" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IY18" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="IZ18" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="19" ht="13.9" customHeight="1" s="3">
@@ -15010,8 +15334,26 @@
       <c r="IS19" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="IT19" t="n">
+      <c r="IT19" s="2" t="n">
         <v>36</v>
+      </c>
+      <c r="IU19" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="IV19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="IW19" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="IX19" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="IY19" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="IZ19" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="20" ht="13.9" customHeight="1" s="3">
@@ -15776,8 +16118,26 @@
       <c r="IS20" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="IT20" t="n">
+      <c r="IT20" s="2" t="n">
         <v>17</v>
+      </c>
+      <c r="IU20" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="IV20" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="IW20" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="IX20" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="IY20" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="IZ20" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="21" ht="13.9" customHeight="1" s="3">
@@ -16542,8 +16902,26 @@
       <c r="IS21" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="IT21" t="n">
+      <c r="IT21" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="IU21" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IV21" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IW21" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IX21" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IY21" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IZ21" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="22" ht="13.9" customHeight="1" s="3">
@@ -17308,8 +17686,26 @@
       <c r="IS22" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="IT22" t="n">
+      <c r="IT22" s="2" t="n">
         <v>9</v>
+      </c>
+      <c r="IU22" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IV22" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IW22" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="IX22" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="IY22" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="IZ22" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="23" ht="13.9" customHeight="1" s="3">
@@ -18074,8 +18470,26 @@
       <c r="IS23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="IT23" t="n">
+      <c r="IT23" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="IU23" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IV23" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="IW23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="IX23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IY23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="IZ23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="13.9" customHeight="1" s="3">
@@ -18840,8 +19254,26 @@
       <c r="IS24" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="IT24" t="n">
+      <c r="IT24" s="2" t="n">
         <v>27</v>
+      </c>
+      <c r="IU24" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="IV24" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="IW24" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="IX24" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="IY24" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="IZ24" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="25" ht="13.9" customHeight="1" s="3">
@@ -19606,8 +20038,26 @@
       <c r="IS25" s="2" t="n">
         <v>72.7</v>
       </c>
-      <c r="IT25" t="n">
+      <c r="IT25" s="2" t="n">
         <v>63</v>
+      </c>
+      <c r="IU25" s="2" t="n">
+        <v>53.3</v>
+      </c>
+      <c r="IV25" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="IW25" s="2" t="n">
+        <v>35.7</v>
+      </c>
+      <c r="IX25" s="2" t="n">
+        <v>38.9</v>
+      </c>
+      <c r="IY25" s="2" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="IZ25" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="26" ht="13.9" customHeight="1" s="3">
@@ -20372,8 +20822,26 @@
       <c r="IS26" s="2" t="n">
         <v>21.44</v>
       </c>
-      <c r="IT26" t="n">
+      <c r="IT26" s="2" t="n">
         <v>20.53</v>
+      </c>
+      <c r="IU26" s="2" t="n">
+        <v>22.69</v>
+      </c>
+      <c r="IV26" s="2" t="n">
+        <v>27.31</v>
+      </c>
+      <c r="IW26" s="2" t="n">
+        <v>36.8</v>
+      </c>
+      <c r="IX26" s="2" t="n">
+        <v>47.43</v>
+      </c>
+      <c r="IY26" s="2" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="IZ26" t="n">
+        <v>23.15</v>
       </c>
     </row>
     <row r="27" ht="13.9" customHeight="1" s="3">
@@ -21138,8 +21606,26 @@
       <c r="IS27" s="2" t="n">
         <v>15.59</v>
       </c>
-      <c r="IT27" t="n">
+      <c r="IT27" s="2" t="n">
         <v>12.93</v>
+      </c>
+      <c r="IU27" s="2" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="IV27" s="2" t="n">
+        <v>17.75</v>
+      </c>
+      <c r="IW27" s="2" t="n">
+        <v>13.14</v>
+      </c>
+      <c r="IX27" s="2" t="n">
+        <v>18.44</v>
+      </c>
+      <c r="IY27" s="2" t="n">
+        <v>12.29</v>
+      </c>
+      <c r="IZ27" t="n">
+        <v>12.04</v>
       </c>
     </row>
     <row r="28" ht="13.9" customHeight="1" s="3">
@@ -21904,8 +22390,26 @@
       <c r="IS28" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="IT28" t="n">
+      <c r="IT28" s="2" t="n">
         <v>42</v>
+      </c>
+      <c r="IU28" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="IV28" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="IW28" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="IX28" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="IY28" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="IZ28" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="29" ht="13.9" customHeight="1" s="3">
@@ -22670,8 +23174,26 @@
       <c r="IS29" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="IT29" t="n">
+      <c r="IT29" s="2" t="n">
         <v>67</v>
+      </c>
+      <c r="IU29" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="IV29" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="IW29" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="IX29" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="IY29" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="IZ29" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="30" ht="13.9" customHeight="1" s="3">
@@ -23436,8 +23958,26 @@
       <c r="IS30" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="IT30" t="n">
+      <c r="IT30" s="2" t="n">
         <v>32</v>
+      </c>
+      <c r="IU30" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="IV30" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="IW30" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="IX30" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="IY30" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="IZ30" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="31" ht="13.9" customHeight="1" s="3">
@@ -24202,8 +24742,26 @@
       <c r="IS31" s="2" t="n">
         <v>57</v>
       </c>
-      <c r="IT31" t="n">
+      <c r="IT31" s="2" t="n">
         <v>61</v>
+      </c>
+      <c r="IU31" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="IV31" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="IW31" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="IX31" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="IY31" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="IZ31" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="32" ht="13.9" customHeight="1" s="3">
@@ -24968,8 +25526,26 @@
       <c r="IS32" s="2" t="n">
         <v>2.59</v>
       </c>
-      <c r="IT32" t="n">
+      <c r="IT32" s="2" t="n">
         <v>2.26</v>
+      </c>
+      <c r="IU32" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="IV32" s="2" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="IW32" s="2" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="IX32" s="2" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="IY32" s="2" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="IZ32" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row r="33" ht="13.9" customHeight="1" s="3">
@@ -25734,8 +26310,26 @@
       <c r="IS33" s="2" t="n">
         <v>3.56</v>
       </c>
-      <c r="IT33" t="n">
+      <c r="IT33" s="2" t="n">
         <v>3.59</v>
+      </c>
+      <c r="IU33" s="2" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="IV33" s="2" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="IW33" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IX33" s="2" t="n">
+        <v>6.14</v>
+      </c>
+      <c r="IY33" s="2" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="IZ33" t="n">
+        <v>3.77</v>
       </c>
     </row>
     <row r="34" ht="13.9" customHeight="1" s="3">
@@ -26500,8 +27094,26 @@
       <c r="IS34" s="2" t="n">
         <v>38.6</v>
       </c>
-      <c r="IT34" t="n">
+      <c r="IT34" s="2" t="n">
         <v>42.6</v>
+      </c>
+      <c r="IU34" s="2" t="n">
+        <v>41.7</v>
+      </c>
+      <c r="IV34" s="2" t="n">
+        <v>31.5</v>
+      </c>
+      <c r="IW34" s="2" t="n">
+        <v>43.3</v>
+      </c>
+      <c r="IX34" s="2" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="IY34" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="IZ34" t="n">
+        <v>46.9</v>
       </c>
     </row>
     <row r="35" ht="13.9" customHeight="1" s="3">
@@ -27266,8 +27878,26 @@
       <c r="IS35" s="2" t="n">
         <v>28.1</v>
       </c>
-      <c r="IT35" t="n">
+      <c r="IT35" s="2" t="n">
         <v>27.9</v>
+      </c>
+      <c r="IU35" s="2" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="IV35" s="2" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="IW35" s="2" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="IX35" s="2" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="IY35" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="IZ35" t="n">
+        <v>26.5</v>
       </c>
     </row>
     <row r="36" ht="13.9" customHeight="1" s="3">
@@ -28032,8 +28662,26 @@
       <c r="IS36" s="2" t="n">
         <v>188.2</v>
       </c>
-      <c r="IT36" t="n">
+      <c r="IT36" s="2" t="n">
         <v>188.4</v>
+      </c>
+      <c r="IU36" s="2" t="n">
+        <v>188</v>
+      </c>
+      <c r="IV36" s="2" t="n">
+        <v>188</v>
+      </c>
+      <c r="IW36" s="2" t="n">
+        <v>188.6</v>
+      </c>
+      <c r="IX36" s="2" t="n">
+        <v>188.5</v>
+      </c>
+      <c r="IY36" s="2" t="n">
+        <v>188.2</v>
+      </c>
+      <c r="IZ36" t="n">
+        <v>189.3</v>
       </c>
     </row>
     <row r="37" ht="13.9" customHeight="1" s="3">
@@ -28798,7 +29446,25 @@
       <c r="IS37" s="2" t="n">
         <v>88.5</v>
       </c>
-      <c r="IT37" t="n">
+      <c r="IT37" s="2" t="n">
+        <v>88.3</v>
+      </c>
+      <c r="IU37" s="2" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="IV37" s="2" t="n">
+        <v>88.09999999999999</v>
+      </c>
+      <c r="IW37" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="IX37" s="2" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="IY37" s="2" t="n">
+        <v>88.09999999999999</v>
+      </c>
+      <c r="IZ37" t="n">
         <v>88.3</v>
       </c>
     </row>
@@ -29564,8 +30230,26 @@
       <c r="IS38" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="IT38" t="n">
+      <c r="IT38" s="2" t="n">
         <v>26.8</v>
+      </c>
+      <c r="IU38" s="2" t="n">
+        <v>26.41</v>
+      </c>
+      <c r="IV38" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="IW38" s="2" t="n">
+        <v>26.74</v>
+      </c>
+      <c r="IX38" s="2" t="n">
+        <v>25.74</v>
+      </c>
+      <c r="IY38" s="2" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="IZ38" t="n">
+        <v>25.66</v>
       </c>
     </row>
     <row r="39" ht="13.9" customHeight="1" s="3">
@@ -30330,8 +31014,26 @@
       <c r="IS39" s="2" t="n">
         <v>103.6</v>
       </c>
-      <c r="IT39" t="n">
+      <c r="IT39" s="2" t="n">
         <v>108.3</v>
+      </c>
+      <c r="IU39" s="2" t="n">
+        <v>112.7</v>
+      </c>
+      <c r="IV39" s="2" t="n">
+        <v>108.4</v>
+      </c>
+      <c r="IW39" s="2" t="n">
+        <v>120.6</v>
+      </c>
+      <c r="IX39" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="IY39" s="2" t="n">
+        <v>110.1</v>
+      </c>
+      <c r="IZ39" t="n">
+        <v>88.2</v>
       </c>
     </row>
     <row r="40" ht="13.9" customHeight="1" s="3">
@@ -31096,8 +31798,26 @@
       <c r="IS40" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="IT40" t="n">
+      <c r="IT40" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="IU40" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IV40" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IW40" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IX40" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IY40" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IZ40" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="41" ht="13.9" customHeight="1" s="3">
@@ -31862,7 +32582,25 @@
       <c r="IS41" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="IT41" t="n">
+      <c r="IT41" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IU41" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="IV41" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="IW41" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IX41" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IY41" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IZ41" t="n">
         <v>6</v>
       </c>
     </row>
@@ -32628,8 +33366,26 @@
       <c r="IS42" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="IT42" t="n">
+      <c r="IT42" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="IU42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IV42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IW42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IX42" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IY42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IZ42" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="43" ht="13.9" customHeight="1" s="3">
@@ -33394,8 +34150,26 @@
       <c r="IS43" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="IT43" t="n">
+      <c r="IT43" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="IU43" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IV43" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IW43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="IX43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="IY43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="IZ43" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="44" ht="13.9" customHeight="1" s="3">
@@ -34160,8 +34934,26 @@
       <c r="IS44" s="2" t="n">
         <v>162</v>
       </c>
-      <c r="IT44" t="n">
+      <c r="IT44" s="2" t="n">
         <v>152</v>
+      </c>
+      <c r="IU44" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="IV44" s="2" t="n">
+        <v>142</v>
+      </c>
+      <c r="IW44" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="IX44" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="IY44" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="IZ44" t="n">
+        <v>127</v>
       </c>
     </row>
     <row r="45" ht="13.9" customHeight="1" s="3">
@@ -34926,8 +35718,26 @@
       <c r="IS45" s="2" t="n">
         <v>167</v>
       </c>
-      <c r="IT45" t="n">
+      <c r="IT45" s="2" t="n">
         <v>198</v>
+      </c>
+      <c r="IU45" s="2" t="n">
+        <v>211</v>
+      </c>
+      <c r="IV45" s="2" t="n">
+        <v>216</v>
+      </c>
+      <c r="IW45" s="2" t="n">
+        <v>233</v>
+      </c>
+      <c r="IX45" s="2" t="n">
+        <v>187</v>
+      </c>
+      <c r="IY45" s="2" t="n">
+        <v>206</v>
+      </c>
+      <c r="IZ45" t="n">
+        <v>164</v>
       </c>
     </row>
     <row r="46" ht="13.9" customHeight="1" s="3">
@@ -35692,8 +36502,26 @@
       <c r="IS46" s="2" t="n">
         <v>237</v>
       </c>
-      <c r="IT46" t="n">
+      <c r="IT46" s="2" t="n">
         <v>257</v>
+      </c>
+      <c r="IU46" s="2" t="n">
+        <v>259</v>
+      </c>
+      <c r="IV46" s="2" t="n">
+        <v>252</v>
+      </c>
+      <c r="IW46" s="2" t="n">
+        <v>267</v>
+      </c>
+      <c r="IX46" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="IY46" s="2" t="n">
+        <v>263</v>
+      </c>
+      <c r="IZ46" t="n">
+        <v>197</v>
       </c>
     </row>
     <row r="47" ht="13.9" customHeight="1" s="3">
@@ -36458,8 +37286,26 @@
       <c r="IS47" s="2" t="n">
         <v>69.09999999999999</v>
       </c>
-      <c r="IT47" t="n">
+      <c r="IT47" s="2" t="n">
         <v>73.59999999999999</v>
+      </c>
+      <c r="IU47" s="2" t="n">
+        <v>71.3</v>
+      </c>
+      <c r="IV47" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="IW47" s="2" t="n">
+        <v>72.59999999999999</v>
+      </c>
+      <c r="IX47" s="2" t="n">
+        <v>69.3</v>
+      </c>
+      <c r="IY47" s="2" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="IZ47" t="n">
+        <v>65.40000000000001</v>
       </c>
     </row>
     <row r="48" ht="13.9" customHeight="1" s="3">
@@ -37224,8 +38070,26 @@
       <c r="IS48" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="IT48" t="n">
+      <c r="IT48" s="2" t="n">
         <v>67</v>
+      </c>
+      <c r="IU48" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="IV48" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="IW48" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="IX48" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="IY48" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="IZ48" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="49" ht="13.9" customHeight="1" s="3">
@@ -37990,7 +38854,25 @@
       <c r="IS49" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="IT49" t="n">
+      <c r="IT49" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="IU49" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IV49" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IW49" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IX49" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="IY49" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="IZ49" t="n">
         <v>13</v>
       </c>
     </row>
@@ -38756,8 +39638,26 @@
       <c r="IS50" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="IT50" t="n">
+      <c r="IT50" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="IU50" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="IV50" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="IW50" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IX50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="IY50" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="IZ50" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="51" ht="13.9" customHeight="1" s="3">
@@ -39522,8 +40422,26 @@
       <c r="IS51" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="IT51" t="n">
+      <c r="IT51" s="2" t="n">
         <v>42</v>
+      </c>
+      <c r="IU51" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="IV51" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="IW51" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="IX51" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="IY51" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="IZ51" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="52" ht="13.9" customHeight="1" s="3">
@@ -40288,8 +41206,26 @@
       <c r="IS52" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="IT52" t="n">
+      <c r="IT52" s="2" t="n">
         <v>32</v>
+      </c>
+      <c r="IU52" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="IV52" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="IW52" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="IX52" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="IY52" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="IZ52" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="53" ht="13.9" customHeight="1" s="3">
@@ -41054,8 +41990,26 @@
       <c r="IS53" s="2" t="n">
         <v>53</v>
       </c>
-      <c r="IT53" t="n">
+      <c r="IT53" s="2" t="n">
         <v>67</v>
+      </c>
+      <c r="IU53" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="IV53" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="IW53" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="IX53" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="IY53" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="IZ53" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="54" ht="13.9" customHeight="1" s="3">
@@ -41820,8 +42774,26 @@
       <c r="IS54" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="IT54" t="n">
+      <c r="IT54" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="IU54" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IV54" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="IW54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IX54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IY54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IZ54" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="55" ht="13.9" customHeight="1" s="3">
@@ -42586,8 +43558,26 @@
       <c r="IS55" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="IT55" t="n">
+      <c r="IT55" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="IU55" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IV55" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IW55" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IX55" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IY55" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IZ55" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="56" ht="13.9" customHeight="1" s="3">
@@ -43352,8 +44342,26 @@
       <c r="IS56" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="IT56" t="n">
+      <c r="IT56" s="2" t="n">
         <v>64.7</v>
+      </c>
+      <c r="IU56" s="2" t="n">
+        <v>68.8</v>
+      </c>
+      <c r="IV56" s="2" t="n">
+        <v>69.2</v>
+      </c>
+      <c r="IW56" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="IX56" s="2" t="n">
+        <v>71.40000000000001</v>
+      </c>
+      <c r="IY56" s="2" t="n">
+        <v>56.2</v>
+      </c>
+      <c r="IZ56" t="n">
+        <v>76.90000000000001</v>
       </c>
     </row>
     <row r="57" ht="13.9" customHeight="1" s="3">
@@ -44118,8 +45126,26 @@
       <c r="IS57" s="2" t="n">
         <v>206</v>
       </c>
-      <c r="IT57" t="n">
+      <c r="IT57" s="2" t="n">
         <v>186</v>
+      </c>
+      <c r="IU57" s="2" t="n">
+        <v>215</v>
+      </c>
+      <c r="IV57" s="2" t="n">
+        <v>218</v>
+      </c>
+      <c r="IW57" s="2" t="n">
+        <v>202</v>
+      </c>
+      <c r="IX57" s="2" t="n">
+        <v>223</v>
+      </c>
+      <c r="IY57" s="2" t="n">
+        <v>198</v>
+      </c>
+      <c r="IZ57" t="n">
+        <v>235</v>
       </c>
     </row>
     <row r="58" ht="13.9" customHeight="1" s="3">
@@ -44884,8 +45910,26 @@
       <c r="IS58" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="IT58" t="n">
+      <c r="IT58" s="2" t="n">
         <v>126</v>
+      </c>
+      <c r="IU58" s="2" t="n">
+        <v>118</v>
+      </c>
+      <c r="IV58" s="2" t="n">
+        <v>166</v>
+      </c>
+      <c r="IW58" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="IX58" s="2" t="n">
+        <v>176</v>
+      </c>
+      <c r="IY58" s="2" t="n">
+        <v>147</v>
+      </c>
+      <c r="IZ58" t="n">
+        <v>147</v>
       </c>
     </row>
     <row r="59" ht="13.9" customHeight="1" s="3">
@@ -45650,8 +46694,26 @@
       <c r="IS59" s="2" t="n">
         <v>353</v>
       </c>
-      <c r="IT59" t="n">
+      <c r="IT59" s="2" t="n">
         <v>312</v>
+      </c>
+      <c r="IU59" s="2" t="n">
+        <v>333</v>
+      </c>
+      <c r="IV59" s="2" t="n">
+        <v>384</v>
+      </c>
+      <c r="IW59" s="2" t="n">
+        <v>325</v>
+      </c>
+      <c r="IX59" s="2" t="n">
+        <v>399</v>
+      </c>
+      <c r="IY59" s="2" t="n">
+        <v>345</v>
+      </c>
+      <c r="IZ59" t="n">
+        <v>382</v>
       </c>
     </row>
     <row r="60" ht="13.9" customHeight="1" s="3">
@@ -46416,8 +47478,26 @@
       <c r="IS60" s="2" t="n">
         <v>1.4</v>
       </c>
-      <c r="IT60" t="n">
+      <c r="IT60" s="2" t="n">
         <v>1.48</v>
+      </c>
+      <c r="IU60" s="2" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="IV60" s="2" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="IW60" s="2" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="IX60" s="2" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="IY60" s="2" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="IZ60" t="n">
+        <v>1.6</v>
       </c>
     </row>
     <row r="61" ht="13.9" customHeight="1" s="3">
@@ -47182,8 +48262,26 @@
       <c r="IS61" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="IT61" t="n">
+      <c r="IT61" s="2" t="n">
         <v>61</v>
+      </c>
+      <c r="IU61" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="IV61" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="IW61" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="IX61" s="2" t="n">
+        <v>84</v>
+      </c>
+      <c r="IY61" s="2" t="n">
+        <v>82</v>
+      </c>
+      <c r="IZ61" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="62" ht="13.9" customHeight="1" s="3">
@@ -47948,8 +49046,26 @@
       <c r="IS62" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="IT62" t="n">
+      <c r="IT62" s="2" t="n">
         <v>62</v>
+      </c>
+      <c r="IU62" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="IV62" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="IW62" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="IX62" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="IY62" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="IZ62" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="63" ht="13.9" customHeight="1" s="3">
@@ -48714,8 +49830,26 @@
       <c r="IS63" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="IT63" t="n">
+      <c r="IT63" s="2" t="n">
         <v>27</v>
+      </c>
+      <c r="IU63" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="IV63" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="IW63" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="IX63" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="IY63" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="IZ63" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="64" ht="13.9" customHeight="1" s="3">
@@ -49480,8 +50614,26 @@
       <c r="IS64" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="IT64" t="n">
+      <c r="IT64" s="2" t="n">
         <v>36</v>
+      </c>
+      <c r="IU64" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="IV64" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="IW64" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="IX64" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="IY64" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="IZ64" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="65" ht="13.9" customHeight="1" s="3">
@@ -50246,8 +51398,26 @@
       <c r="IS65" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="IT65" t="n">
+      <c r="IT65" s="2" t="n">
         <v>27</v>
+      </c>
+      <c r="IU65" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="IV65" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="IW65" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="IX65" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IY65" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="IZ65" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="66" ht="13.9" customHeight="1" s="3">
@@ -51012,8 +52182,26 @@
       <c r="IS66" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="IT66" t="n">
+      <c r="IT66" s="2" t="n">
         <v>18</v>
+      </c>
+      <c r="IU66" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="IV66" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="IW66" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="IX66" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="IY66" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IZ66" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="67" ht="13.9" customHeight="1" s="3">
@@ -51778,8 +52966,26 @@
       <c r="IS67" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="IT67" t="n">
+      <c r="IT67" s="2" t="n">
         <v>9</v>
+      </c>
+      <c r="IU67" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="IV67" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IW67" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IX67" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IY67" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IZ67" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="68" ht="13.9" customHeight="1" s="3">
@@ -52544,8 +53750,26 @@
       <c r="IS68" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="IT68" t="n">
+      <c r="IT68" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="IU68" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IV68" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IW68" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="IX68" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="IY68" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IZ68" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="69" ht="13.9" customHeight="1" s="3">
@@ -53310,8 +54534,26 @@
       <c r="IS69" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IT69" t="n">
+      <c r="IT69" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="IU69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IV69" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IW69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IX69" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="IY69" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IZ69" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="70" ht="13.9" customHeight="1" s="3">
@@ -54076,8 +55318,26 @@
       <c r="IS70" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="IT70" t="n">
+      <c r="IT70" s="2" t="n">
         <v>27</v>
+      </c>
+      <c r="IU70" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="IV70" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="IW70" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="IX70" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="IY70" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="IZ70" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="71" ht="13.9" customHeight="1" s="3">
@@ -54842,8 +56102,26 @@
       <c r="IS71" s="2" t="n">
         <v>42.9</v>
       </c>
-      <c r="IT71" t="n">
+      <c r="IT71" s="2" t="n">
         <v>66.7</v>
+      </c>
+      <c r="IU71" s="2" t="n">
+        <v>71.40000000000001</v>
+      </c>
+      <c r="IV71" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="IW71" s="2" t="n">
+        <v>47.1</v>
+      </c>
+      <c r="IX71" s="2" t="n">
+        <v>43.2</v>
+      </c>
+      <c r="IY71" s="2" t="n">
+        <v>40.9</v>
+      </c>
+      <c r="IZ71" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="72" ht="13.9" customHeight="1" s="3">
@@ -55608,8 +56886,26 @@
       <c r="IS72" s="2" t="n">
         <v>39.22</v>
       </c>
-      <c r="IT72" t="n">
+      <c r="IT72" s="2" t="n">
         <v>17.33</v>
+      </c>
+      <c r="IU72" s="2" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="IV72" s="2" t="n">
+        <v>25.6</v>
+      </c>
+      <c r="IW72" s="2" t="n">
+        <v>40.62</v>
+      </c>
+      <c r="IX72" s="2" t="n">
+        <v>24.94</v>
+      </c>
+      <c r="IY72" s="2" t="n">
+        <v>38.33</v>
+      </c>
+      <c r="IZ72" t="n">
+        <v>25.47</v>
       </c>
     </row>
     <row r="73" ht="13.9" customHeight="1" s="3">
@@ -56374,8 +57670,26 @@
       <c r="IS73" s="2" t="n">
         <v>16.81</v>
       </c>
-      <c r="IT73" t="n">
+      <c r="IT73" s="2" t="n">
         <v>11.56</v>
+      </c>
+      <c r="IU73" s="2" t="n">
+        <v>15.86</v>
+      </c>
+      <c r="IV73" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="IW73" s="2" t="n">
+        <v>19.12</v>
+      </c>
+      <c r="IX73" s="2" t="n">
+        <v>10.78</v>
+      </c>
+      <c r="IY73" s="2" t="n">
+        <v>15.68</v>
+      </c>
+      <c r="IZ73" t="n">
+        <v>15.28</v>
       </c>
     </row>
     <row r="74" ht="13.9" customHeight="1" s="3">
@@ -57140,8 +58454,26 @@
       <c r="IS74" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="IT74" t="n">
+      <c r="IT74" s="2" t="n">
         <v>43</v>
+      </c>
+      <c r="IU74" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="IV74" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="IW74" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="IX74" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="IY74" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="IZ74" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="75" ht="13.9" customHeight="1" s="3">
@@ -57906,8 +59238,26 @@
       <c r="IS75" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="IT75" t="n">
+      <c r="IT75" s="2" t="n">
         <v>63</v>
+      </c>
+      <c r="IU75" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="IV75" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="IW75" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="IX75" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="IY75" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="IZ75" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="76" ht="13.9" customHeight="1" s="3">
@@ -58672,8 +60022,26 @@
       <c r="IS76" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="IT76" t="n">
+      <c r="IT76" s="2" t="n">
         <v>43</v>
+      </c>
+      <c r="IU76" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="IV76" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="IW76" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="IX76" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="IY76" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="IZ76" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="77" ht="13.9" customHeight="1" s="3">
@@ -59438,8 +60806,26 @@
       <c r="IS77" s="2" t="n">
         <v>53</v>
       </c>
-      <c r="IT77" t="n">
+      <c r="IT77" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="IU77" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="IV77" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="IW77" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="IX77" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="IY77" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="IZ77" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="78" ht="13.9" customHeight="1" s="3">
@@ -60204,8 +61590,26 @@
       <c r="IS78" s="2" t="n">
         <v>2.52</v>
       </c>
-      <c r="IT78" t="n">
+      <c r="IT78" s="2" t="n">
         <v>1.85</v>
+      </c>
+      <c r="IU78" s="2" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="IV78" s="2" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="IW78" s="2" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="IX78" s="2" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="IY78" s="2" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="IZ78" t="n">
+        <v>2.24</v>
       </c>
     </row>
     <row r="79" ht="13.9" customHeight="1" s="3">
@@ -60970,8 +62374,26 @@
       <c r="IS79" s="2" t="n">
         <v>5.89</v>
       </c>
-      <c r="IT79" t="n">
+      <c r="IT79" s="2" t="n">
         <v>2.78</v>
+      </c>
+      <c r="IU79" s="2" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="IV79" s="2" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="IW79" s="2" t="n">
+        <v>5.12</v>
+      </c>
+      <c r="IX79" s="2" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="IY79" s="2" t="n">
+        <v>6.33</v>
+      </c>
+      <c r="IZ79" t="n">
+        <v>3.73</v>
       </c>
     </row>
     <row r="80" ht="13.9" customHeight="1" s="3">
@@ -61736,8 +63158,26 @@
       <c r="IS80" s="2" t="n">
         <v>37.7</v>
       </c>
-      <c r="IT80" t="n">
+      <c r="IT80" s="2" t="n">
         <v>44</v>
+      </c>
+      <c r="IU80" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="IV80" s="2" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="IW80" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="IX80" s="2" t="n">
+        <v>48.4</v>
+      </c>
+      <c r="IY80" s="2" t="n">
+        <v>31.6</v>
+      </c>
+      <c r="IZ80" t="n">
+        <v>42.9</v>
       </c>
     </row>
     <row r="81" ht="13.9" customHeight="1" s="3">
@@ -62502,8 +63942,26 @@
       <c r="IS81" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="IT81" t="n">
+      <c r="IT81" s="2" t="n">
         <v>36</v>
+      </c>
+      <c r="IU81" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="IV81" s="2" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="IW81" s="2" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="IX81" s="2" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="IY81" s="2" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="IZ81" t="n">
+        <v>26.8</v>
       </c>
     </row>
     <row r="82" ht="13.9" customHeight="1" s="3">
@@ -63268,8 +64726,26 @@
       <c r="IS82" s="2" t="n">
         <v>186.7</v>
       </c>
-      <c r="IT82" t="n">
+      <c r="IT82" s="2" t="n">
         <v>187.2</v>
+      </c>
+      <c r="IU82" s="2" t="n">
+        <v>189.2</v>
+      </c>
+      <c r="IV82" s="2" t="n">
+        <v>188.6</v>
+      </c>
+      <c r="IW82" s="2" t="n">
+        <v>188.2</v>
+      </c>
+      <c r="IX82" s="2" t="n">
+        <v>186.1</v>
+      </c>
+      <c r="IY82" s="2" t="n">
+        <v>188.8</v>
+      </c>
+      <c r="IZ82" t="n">
+        <v>188.3</v>
       </c>
     </row>
     <row r="83" ht="13.9" customHeight="1" s="3">
@@ -64034,8 +65510,26 @@
       <c r="IS83" s="2" t="n">
         <v>86.2</v>
       </c>
-      <c r="IT83" t="n">
+      <c r="IT83" s="2" t="n">
         <v>85.59999999999999</v>
+      </c>
+      <c r="IU83" s="2" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="IV83" s="2" t="n">
+        <v>89.5</v>
+      </c>
+      <c r="IW83" s="2" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="IX83" s="2" t="n">
+        <v>85.7</v>
+      </c>
+      <c r="IY83" s="2" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="IZ83" t="n">
+        <v>85.90000000000001</v>
       </c>
     </row>
     <row r="84" ht="13.9" customHeight="1" s="3">
@@ -64800,8 +66294,26 @@
       <c r="IS84" s="2" t="n">
         <v>24.16</v>
       </c>
-      <c r="IT84" t="n">
+      <c r="IT84" s="2" t="n">
         <v>25.24</v>
+      </c>
+      <c r="IU84" s="2" t="n">
+        <v>24.91</v>
+      </c>
+      <c r="IV84" s="2" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="IW84" s="2" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="IX84" s="2" t="n">
+        <v>25.24</v>
+      </c>
+      <c r="IY84" s="2" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="IZ84" t="n">
+        <v>24.8</v>
       </c>
     </row>
     <row r="85" ht="13.9" customHeight="1" s="3">
@@ -65566,8 +67078,26 @@
       <c r="IS85" s="2" t="n">
         <v>63.1</v>
       </c>
-      <c r="IT85" t="n">
+      <c r="IT85" s="2" t="n">
         <v>88</v>
+      </c>
+      <c r="IU85" s="2" t="n">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="IV85" s="2" t="n">
+        <v>80.90000000000001</v>
+      </c>
+      <c r="IW85" s="2" t="n">
+        <v>97.90000000000001</v>
+      </c>
+      <c r="IX85" s="2" t="n">
+        <v>100.2</v>
+      </c>
+      <c r="IY85" s="2" t="n">
+        <v>90.40000000000001</v>
+      </c>
+      <c r="IZ85" t="n">
+        <v>77.2</v>
       </c>
     </row>
     <row r="86" ht="13.9" customHeight="1" s="3">
@@ -66332,8 +67862,26 @@
       <c r="IS86" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="IT86" t="n">
+      <c r="IT86" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="IU86" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="IV86" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="IW86" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IX86" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IY86" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IZ86" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="87" ht="13.9" customHeight="1" s="3">
@@ -67098,8 +68646,26 @@
       <c r="IS87" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="IT87" t="n">
+      <c r="IT87" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="IU87" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="IV87" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IW87" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="IX87" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IY87" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IZ87" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="88" ht="13.9" customHeight="1" s="3">
@@ -67864,8 +69430,26 @@
       <c r="IS88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="IT88" t="n">
+      <c r="IT88" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="IU88" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="IV88" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IW88" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IX88" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IY88" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IZ88" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="89" ht="13.9" customHeight="1" s="3">
@@ -68630,7 +70214,25 @@
       <c r="IS89" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="IT89" t="n">
+      <c r="IT89" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IU89" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IV89" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="IW89" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="IX89" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IY89" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="IZ89" t="n">
         <v>4</v>
       </c>
     </row>
@@ -69396,8 +70998,26 @@
       <c r="IS90" s="2" t="n">
         <v>149</v>
       </c>
-      <c r="IT90" t="n">
+      <c r="IT90" s="2" t="n">
         <v>142</v>
+      </c>
+      <c r="IU90" s="2" t="n">
+        <v>126</v>
+      </c>
+      <c r="IV90" s="2" t="n">
+        <v>139</v>
+      </c>
+      <c r="IW90" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="IX90" s="2" t="n">
+        <v>170</v>
+      </c>
+      <c r="IY90" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="IZ90" t="n">
+        <v>137</v>
       </c>
     </row>
     <row r="91" ht="13.9" customHeight="1" s="3">
@@ -70162,8 +71782,26 @@
       <c r="IS91" s="2" t="n">
         <v>195</v>
       </c>
-      <c r="IT91" t="n">
+      <c r="IT91" s="2" t="n">
         <v>169</v>
+      </c>
+      <c r="IU91" s="2" t="n">
+        <v>199</v>
+      </c>
+      <c r="IV91" s="2" t="n">
+        <v>246</v>
+      </c>
+      <c r="IW91" s="2" t="n">
+        <v>197</v>
+      </c>
+      <c r="IX91" s="2" t="n">
+        <v>232</v>
+      </c>
+      <c r="IY91" s="2" t="n">
+        <v>210</v>
+      </c>
+      <c r="IZ91" t="n">
+        <v>237</v>
       </c>
     </row>
     <row r="92" ht="13.9" customHeight="1" s="3">
@@ -70928,8 +72566,26 @@
       <c r="IS92" s="2" t="n">
         <v>256</v>
       </c>
-      <c r="IT92" t="n">
+      <c r="IT92" s="2" t="n">
         <v>229</v>
+      </c>
+      <c r="IU92" s="2" t="n">
+        <v>242</v>
+      </c>
+      <c r="IV92" s="2" t="n">
+        <v>292</v>
+      </c>
+      <c r="IW92" s="2" t="n">
+        <v>235</v>
+      </c>
+      <c r="IX92" s="2" t="n">
+        <v>283</v>
+      </c>
+      <c r="IY92" s="2" t="n">
+        <v>241</v>
+      </c>
+      <c r="IZ92" t="n">
+        <v>287</v>
       </c>
     </row>
     <row r="93" ht="13.9" customHeight="1" s="3">
@@ -71694,8 +73350,26 @@
       <c r="IS93" s="2" t="n">
         <v>72.5</v>
       </c>
-      <c r="IT93" t="n">
+      <c r="IT93" s="2" t="n">
         <v>73.40000000000001</v>
+      </c>
+      <c r="IU93" s="2" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="IV93" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="IW93" s="2" t="n">
+        <v>72.3</v>
+      </c>
+      <c r="IX93" s="2" t="n">
+        <v>70.90000000000001</v>
+      </c>
+      <c r="IY93" s="2" t="n">
+        <v>69.90000000000001</v>
+      </c>
+      <c r="IZ93" t="n">
+        <v>75.09999999999999</v>
       </c>
     </row>
     <row r="94" ht="13.9" customHeight="1" s="3">
@@ -72460,8 +74134,26 @@
       <c r="IS94" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="IT94" t="n">
+      <c r="IT94" s="2" t="n">
         <v>63</v>
+      </c>
+      <c r="IU94" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="IV94" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="IW94" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="IX94" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="IY94" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="IZ94" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="95" ht="13.9" customHeight="1" s="3">
@@ -73226,8 +74918,26 @@
       <c r="IS95" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="IT95" t="n">
+      <c r="IT95" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="IU95" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="IV95" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="IW95" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="IX95" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IY95" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IZ95" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="96" ht="13.9" customHeight="1" s="3">
@@ -73992,8 +75702,26 @@
       <c r="IS96" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="IT96" t="n">
+      <c r="IT96" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="IU96" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="IV96" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IW96" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="IX96" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="IY96" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="IZ96" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="97" ht="13.9" customHeight="1" s="3">
@@ -74758,8 +76486,26 @@
       <c r="IS97" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="IT97" t="n">
+      <c r="IT97" s="2" t="n">
         <v>43</v>
+      </c>
+      <c r="IU97" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="IV97" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="IW97" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="IX97" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="IY97" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="IZ97" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="98" ht="13.9" customHeight="1" s="3">
@@ -75524,8 +77270,26 @@
       <c r="IS98" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="IT98" t="n">
+      <c r="IT98" s="2" t="n">
         <v>43</v>
+      </c>
+      <c r="IU98" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="IV98" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="IW98" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="IX98" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="IY98" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="IZ98" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="99" ht="13.9" customHeight="1" s="3">
@@ -76290,8 +78054,26 @@
       <c r="IS99" s="2" t="n">
         <v>51</v>
       </c>
-      <c r="IT99" t="n">
+      <c r="IT99" s="2" t="n">
         <v>56</v>
+      </c>
+      <c r="IU99" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="IV99" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="IW99" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="IX99" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="IY99" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="IZ99" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="100" ht="13.9" customHeight="1" s="3">
@@ -77056,8 +78838,26 @@
       <c r="IS100" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IT100" t="n">
+      <c r="IT100" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="IU100" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IV100" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="IW100" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IX100" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="IY100" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="IZ100" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="101" ht="13.9" customHeight="1" s="3">
@@ -77822,8 +79622,26 @@
       <c r="IS101" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="IT101" t="n">
+      <c r="IT101" s="2" t="n">
         <v>9</v>
+      </c>
+      <c r="IU101" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="IV101" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="IW101" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="IX101" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="IY101" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="IZ101" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="102" ht="13.9" customHeight="1" s="3">
@@ -78588,8 +80406,26 @@
       <c r="IS102" s="2" t="n">
         <v>77.8</v>
       </c>
-      <c r="IT102" t="n">
+      <c r="IT102" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="IU102" s="2" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="IV102" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="IW102" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="IX102" s="2" t="n">
+        <v>68.8</v>
+      </c>
+      <c r="IY102" s="2" t="n">
+        <v>55.6</v>
+      </c>
+      <c r="IZ102" t="n">
+        <v>73.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PF predictions and minor R updates to work with finals gathering
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Brisbane_stats.xlsx
+++ b/django_AFL_ML/Data/Brisbane_stats.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JK102"/>
+  <dimension ref="A1:JN102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="HZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="IL36" activeCellId="0" sqref="IL36"/>
@@ -1273,8 +1273,17 @@
       <c r="JJ1" s="2" t="n">
         <v>10728</v>
       </c>
-      <c r="JK1" t="n">
+      <c r="JK1" s="2" t="n">
         <v>10733</v>
+      </c>
+      <c r="JL1" s="2" t="n">
+        <v>10742</v>
+      </c>
+      <c r="JM1" s="2" t="n">
+        <v>10742</v>
+      </c>
+      <c r="JN1" t="n">
+        <v>10746</v>
       </c>
     </row>
     <row r="2" ht="13.9" customHeight="1" s="3">
@@ -2090,7 +2099,16 @@
       <c r="JJ2" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="JK2" t="n">
+      <c r="JK2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JL2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JM2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JN2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2907,8 +2925,17 @@
       <c r="JJ3" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="JK3" t="n">
+      <c r="JK3" s="2" t="n">
         <v>23</v>
+      </c>
+      <c r="JL3" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="JM3" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="JN3" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="4" ht="13.9" customHeight="1" s="3">
@@ -3724,8 +3751,17 @@
       <c r="JJ4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="JK4" t="n">
+      <c r="JK4" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="JL4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JM4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JN4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.9" customHeight="1" s="3">
@@ -4541,7 +4577,16 @@
       <c r="JJ5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="JK5" t="n">
+      <c r="JK5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JL5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JM5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JN5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5358,8 +5403,17 @@
       <c r="JJ6" s="2" t="n">
         <v>81</v>
       </c>
-      <c r="JK6" t="n">
+      <c r="JK6" s="2" t="n">
         <v>57</v>
+      </c>
+      <c r="JL6" s="2" t="n">
+        <v>106</v>
+      </c>
+      <c r="JM6" s="2" t="n">
+        <v>106</v>
+      </c>
+      <c r="JN6" t="n">
+        <v>92</v>
       </c>
     </row>
     <row r="7" ht="13.9" customHeight="1" s="3">
@@ -6175,8 +6229,17 @@
       <c r="JJ7" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="JK7" t="n">
+      <c r="JK7" s="2" t="n">
         <v>115</v>
+      </c>
+      <c r="JL7" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="JM7" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="JN7" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="8" ht="13.9" customHeight="1" s="3">
@@ -6992,8 +7055,17 @@
       <c r="JJ8" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="JK8" t="n">
+      <c r="JK8" s="2" t="n">
         <v>-58</v>
+      </c>
+      <c r="JL8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JM8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JN8" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="9" ht="13.9" customHeight="1" s="3">
@@ -7809,8 +7881,17 @@
       <c r="JJ9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="JK9" t="n">
+      <c r="JK9" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="JL9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JM9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JN9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="13.9" customHeight="1" s="3">
@@ -8626,7 +8707,16 @@
       <c r="JJ10" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="JK10" t="n">
+      <c r="JK10" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JL10" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="JM10" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="JN10" t="n">
         <v>11</v>
       </c>
     </row>
@@ -9443,8 +9533,17 @@
       <c r="JJ11" s="2" t="n">
         <v>205</v>
       </c>
-      <c r="JK11" t="n">
+      <c r="JK11" s="2" t="n">
         <v>225</v>
+      </c>
+      <c r="JL11" s="2" t="n">
+        <v>210</v>
+      </c>
+      <c r="JM11" s="2" t="n">
+        <v>210</v>
+      </c>
+      <c r="JN11" t="n">
+        <v>229</v>
       </c>
     </row>
     <row r="12" ht="13.9" customHeight="1" s="3">
@@ -10260,8 +10359,17 @@
       <c r="JJ12" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="JK12" t="n">
+      <c r="JK12" s="2" t="n">
         <v>123</v>
+      </c>
+      <c r="JL12" s="2" t="n">
+        <v>126</v>
+      </c>
+      <c r="JM12" s="2" t="n">
+        <v>126</v>
+      </c>
+      <c r="JN12" t="n">
+        <v>111</v>
       </c>
     </row>
     <row r="13" ht="13.9" customHeight="1" s="3">
@@ -11077,8 +11185,17 @@
       <c r="JJ13" s="2" t="n">
         <v>310</v>
       </c>
-      <c r="JK13" t="n">
+      <c r="JK13" s="2" t="n">
         <v>348</v>
+      </c>
+      <c r="JL13" s="2" t="n">
+        <v>336</v>
+      </c>
+      <c r="JM13" s="2" t="n">
+        <v>336</v>
+      </c>
+      <c r="JN13" t="n">
+        <v>340</v>
       </c>
     </row>
     <row r="14" ht="13.9" customHeight="1" s="3">
@@ -11894,8 +12011,17 @@
       <c r="JJ14" s="2" t="n">
         <v>1.95</v>
       </c>
-      <c r="JK14" t="n">
+      <c r="JK14" s="2" t="n">
         <v>1.83</v>
+      </c>
+      <c r="JL14" s="2" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="JM14" s="2" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="JN14" t="n">
+        <v>2.06</v>
       </c>
     </row>
     <row r="15" ht="13.9" customHeight="1" s="3">
@@ -12711,8 +12837,17 @@
       <c r="JJ15" s="2" t="n">
         <v>87</v>
       </c>
-      <c r="JK15" t="n">
+      <c r="JK15" s="2" t="n">
         <v>108</v>
+      </c>
+      <c r="JL15" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="JM15" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="JN15" t="n">
+        <v>92</v>
       </c>
     </row>
     <row r="16" ht="13.9" customHeight="1" s="3">
@@ -13528,8 +13663,17 @@
       <c r="JJ16" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="JK16" t="n">
+      <c r="JK16" s="2" t="n">
         <v>52</v>
+      </c>
+      <c r="JL16" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="JM16" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="JN16" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="17" ht="13.9" customHeight="1" s="3">
@@ -14345,8 +14489,17 @@
       <c r="JJ17" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="JK17" t="n">
+      <c r="JK17" s="2" t="n">
         <v>34</v>
+      </c>
+      <c r="JL17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="JM17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="JN17" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="18" ht="13.9" customHeight="1" s="3">
@@ -15162,8 +15315,17 @@
       <c r="JJ18" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="JK18" t="n">
+      <c r="JK18" s="2" t="n">
         <v>16</v>
+      </c>
+      <c r="JL18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JM18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JN18" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="19" ht="13.9" customHeight="1" s="3">
@@ -15979,8 +16141,17 @@
       <c r="JJ19" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="JK19" t="n">
+      <c r="JK19" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="JL19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="JM19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="JN19" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="20" ht="13.9" customHeight="1" s="3">
@@ -16796,8 +16967,17 @@
       <c r="JJ20" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="JK20" t="n">
+      <c r="JK20" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="JL20" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="JM20" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="JN20" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="21" ht="13.9" customHeight="1" s="3">
@@ -17613,8 +17793,17 @@
       <c r="JJ21" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="JK21" t="n">
+      <c r="JK21" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="JL21" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JM21" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JN21" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="22" ht="13.9" customHeight="1" s="3">
@@ -18430,7 +18619,16 @@
       <c r="JJ22" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JK22" t="n">
+      <c r="JK22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JL22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JM22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JN22" t="n">
         <v>7</v>
       </c>
     </row>
@@ -19247,8 +19445,17 @@
       <c r="JJ23" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="JK23" t="n">
+      <c r="JK23" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="JL23" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JM23" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JN23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" ht="13.9" customHeight="1" s="3">
@@ -20064,8 +20271,17 @@
       <c r="JJ24" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="JK24" t="n">
+      <c r="JK24" s="2" t="n">
         <v>17</v>
+      </c>
+      <c r="JL24" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="JM24" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="JN24" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="25" ht="13.9" customHeight="1" s="3">
@@ -20881,8 +21097,17 @@
       <c r="JJ25" s="2" t="n">
         <v>57.1</v>
       </c>
-      <c r="JK25" t="n">
+      <c r="JK25" s="2" t="n">
         <v>47.1</v>
+      </c>
+      <c r="JL25" s="2" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="JM25" s="2" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="JN25" t="n">
+        <v>63.6</v>
       </c>
     </row>
     <row r="26" ht="13.9" customHeight="1" s="3">
@@ -21698,8 +21923,17 @@
       <c r="JJ26" s="2" t="n">
         <v>25.83</v>
       </c>
-      <c r="JK26" t="n">
+      <c r="JK26" s="2" t="n">
         <v>43.5</v>
+      </c>
+      <c r="JL26" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="JM26" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="JN26" t="n">
+        <v>24.29</v>
       </c>
     </row>
     <row r="27" ht="13.9" customHeight="1" s="3">
@@ -22515,8 +22749,17 @@
       <c r="JJ27" s="2" t="n">
         <v>14.76</v>
       </c>
-      <c r="JK27" t="n">
+      <c r="JK27" s="2" t="n">
         <v>20.47</v>
+      </c>
+      <c r="JL27" s="2" t="n">
+        <v>12.92</v>
+      </c>
+      <c r="JM27" s="2" t="n">
+        <v>12.92</v>
+      </c>
+      <c r="JN27" t="n">
+        <v>15.45</v>
       </c>
     </row>
     <row r="28" ht="13.9" customHeight="1" s="3">
@@ -23332,8 +23575,17 @@
       <c r="JJ28" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="JK28" t="n">
+      <c r="JK28" s="2" t="n">
         <v>36</v>
+      </c>
+      <c r="JL28" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="JM28" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="JN28" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="29" ht="13.9" customHeight="1" s="3">
@@ -24149,8 +24401,17 @@
       <c r="JJ29" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="JK29" t="n">
+      <c r="JK29" s="2" t="n">
         <v>54</v>
+      </c>
+      <c r="JL29" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="JM29" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="JN29" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="30" ht="13.9" customHeight="1" s="3">
@@ -24966,8 +25227,17 @@
       <c r="JJ30" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="JK30" t="n">
+      <c r="JK30" s="2" t="n">
         <v>31</v>
+      </c>
+      <c r="JL30" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JM30" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JN30" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="31" ht="13.9" customHeight="1" s="3">
@@ -25783,8 +26053,17 @@
       <c r="JJ31" s="2" t="n">
         <v>49</v>
       </c>
-      <c r="JK31" t="n">
+      <c r="JK31" s="2" t="n">
         <v>58</v>
+      </c>
+      <c r="JL31" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="JM31" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="JN31" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="32" ht="13.9" customHeight="1" s="3">
@@ -26600,8 +26879,17 @@
       <c r="JJ32" s="2" t="n">
         <v>2.33</v>
       </c>
-      <c r="JK32" t="n">
+      <c r="JK32" s="2" t="n">
         <v>3.41</v>
+      </c>
+      <c r="JL32" s="2" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="JM32" s="2" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="JN32" t="n">
+        <v>2.41</v>
       </c>
     </row>
     <row r="33" ht="13.9" customHeight="1" s="3">
@@ -27417,8 +27705,17 @@
       <c r="JJ33" s="2" t="n">
         <v>4.08</v>
       </c>
-      <c r="JK33" t="n">
+      <c r="JK33" s="2" t="n">
         <v>7.25</v>
+      </c>
+      <c r="JL33" s="2" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="JM33" s="2" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="JN33" t="n">
+        <v>3.79</v>
       </c>
     </row>
     <row r="34" ht="13.9" customHeight="1" s="3">
@@ -28234,8 +28531,17 @@
       <c r="JJ34" s="2" t="n">
         <v>34.7</v>
       </c>
-      <c r="JK34" t="n">
+      <c r="JK34" s="2" t="n">
         <v>25.9</v>
+      </c>
+      <c r="JL34" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JM34" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JN34" t="n">
+        <v>39.6</v>
       </c>
     </row>
     <row r="35" ht="13.9" customHeight="1" s="3">
@@ -29051,8 +29357,17 @@
       <c r="JJ35" s="2" t="n">
         <v>24.5</v>
       </c>
-      <c r="JK35" t="n">
+      <c r="JK35" s="2" t="n">
         <v>13.8</v>
+      </c>
+      <c r="JL35" s="2" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="JM35" s="2" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="JN35" t="n">
+        <v>26.4</v>
       </c>
     </row>
     <row r="36" ht="13.9" customHeight="1" s="3">
@@ -29868,8 +30183,17 @@
       <c r="JJ36" s="2" t="n">
         <v>188.5</v>
       </c>
-      <c r="JK36" t="n">
+      <c r="JK36" s="2" t="n">
         <v>188.2</v>
+      </c>
+      <c r="JL36" s="2" t="n">
+        <v>188.1</v>
+      </c>
+      <c r="JM36" s="2" t="n">
+        <v>188.1</v>
+      </c>
+      <c r="JN36" t="n">
+        <v>187.9</v>
       </c>
     </row>
     <row r="37" ht="13.9" customHeight="1" s="3">
@@ -30685,8 +31009,17 @@
       <c r="JJ37" s="2" t="n">
         <v>88.5</v>
       </c>
-      <c r="JK37" t="n">
+      <c r="JK37" s="2" t="n">
         <v>88.7</v>
+      </c>
+      <c r="JL37" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="JM37" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="JN37" t="n">
+        <v>87.3</v>
       </c>
     </row>
     <row r="38" ht="13.9" customHeight="1" s="3">
@@ -31502,8 +31835,17 @@
       <c r="JJ38" s="2" t="n">
         <v>26.33</v>
       </c>
-      <c r="JK38" t="n">
+      <c r="JK38" s="2" t="n">
         <v>26.49</v>
+      </c>
+      <c r="JL38" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="JM38" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="JN38" t="n">
+        <v>25.49</v>
       </c>
     </row>
     <row r="39" ht="13.9" customHeight="1" s="3">
@@ -32319,8 +32661,17 @@
       <c r="JJ39" s="2" t="n">
         <v>123.5</v>
       </c>
-      <c r="JK39" t="n">
+      <c r="JK39" s="2" t="n">
         <v>128.2</v>
+      </c>
+      <c r="JL39" s="2" t="n">
+        <v>120.9</v>
+      </c>
+      <c r="JM39" s="2" t="n">
+        <v>120.9</v>
+      </c>
+      <c r="JN39" t="n">
+        <v>106.7</v>
       </c>
     </row>
     <row r="40" ht="13.9" customHeight="1" s="3">
@@ -33136,8 +33487,17 @@
       <c r="JJ40" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="JK40" t="n">
+      <c r="JK40" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="JL40" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JM40" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JN40" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="41" ht="13.9" customHeight="1" s="3">
@@ -33953,7 +34313,16 @@
       <c r="JJ41" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JK41" t="n">
+      <c r="JK41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JL41" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JM41" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JN41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -34770,7 +35139,16 @@
       <c r="JJ42" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JK42" t="n">
+      <c r="JK42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JL42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JM42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JN42" t="n">
         <v>5</v>
       </c>
     </row>
@@ -35587,8 +35965,17 @@
       <c r="JJ43" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="JK43" t="n">
+      <c r="JK43" s="2" t="n">
         <v>9</v>
+      </c>
+      <c r="JL43" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JM43" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JN43" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="44" ht="13.9" customHeight="1" s="3">
@@ -36404,8 +36791,17 @@
       <c r="JJ44" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="JK44" t="n">
+      <c r="JK44" s="2" t="n">
         <v>130</v>
+      </c>
+      <c r="JL44" s="2" t="n">
+        <v>149</v>
+      </c>
+      <c r="JM44" s="2" t="n">
+        <v>149</v>
+      </c>
+      <c r="JN44" t="n">
+        <v>137</v>
       </c>
     </row>
     <row r="45" ht="13.9" customHeight="1" s="3">
@@ -37221,8 +37617,17 @@
       <c r="JJ45" s="2" t="n">
         <v>179</v>
       </c>
-      <c r="JK45" t="n">
+      <c r="JK45" s="2" t="n">
         <v>207</v>
+      </c>
+      <c r="JL45" s="2" t="n">
+        <v>182</v>
+      </c>
+      <c r="JM45" s="2" t="n">
+        <v>182</v>
+      </c>
+      <c r="JN45" t="n">
+        <v>194</v>
       </c>
     </row>
     <row r="46" ht="13.9" customHeight="1" s="3">
@@ -38038,8 +38443,17 @@
       <c r="JJ46" s="2" t="n">
         <v>218</v>
       </c>
-      <c r="JK46" t="n">
+      <c r="JK46" s="2" t="n">
         <v>245</v>
+      </c>
+      <c r="JL46" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JM46" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JN46" t="n">
+        <v>229</v>
       </c>
     </row>
     <row r="47" ht="13.9" customHeight="1" s="3">
@@ -38855,8 +39269,17 @@
       <c r="JJ47" s="2" t="n">
         <v>70.3</v>
       </c>
-      <c r="JK47" t="n">
+      <c r="JK47" s="2" t="n">
         <v>70.40000000000001</v>
+      </c>
+      <c r="JL47" s="2" t="n">
+        <v>68.2</v>
+      </c>
+      <c r="JM47" s="2" t="n">
+        <v>68.2</v>
+      </c>
+      <c r="JN47" t="n">
+        <v>67.40000000000001</v>
       </c>
     </row>
     <row r="48" ht="13.9" customHeight="1" s="3">
@@ -39672,8 +40095,17 @@
       <c r="JJ48" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="JK48" t="n">
+      <c r="JK48" s="2" t="n">
         <v>54</v>
+      </c>
+      <c r="JL48" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="JM48" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="JN48" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="49" ht="13.9" customHeight="1" s="3">
@@ -40489,8 +40921,17 @@
       <c r="JJ49" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="JK49" t="n">
+      <c r="JK49" s="2" t="n">
         <v>9</v>
+      </c>
+      <c r="JL49" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JM49" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JN49" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="50" ht="13.9" customHeight="1" s="3">
@@ -41306,8 +41747,17 @@
       <c r="JJ50" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="JK50" t="n">
+      <c r="JK50" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="JL50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JM50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JN50" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="51" ht="13.9" customHeight="1" s="3">
@@ -42123,8 +42573,17 @@
       <c r="JJ51" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="JK51" t="n">
+      <c r="JK51" s="2" t="n">
         <v>36</v>
+      </c>
+      <c r="JL51" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="JM51" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="JN51" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="52" ht="13.9" customHeight="1" s="3">
@@ -42940,8 +43399,17 @@
       <c r="JJ52" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="JK52" t="n">
+      <c r="JK52" s="2" t="n">
         <v>31</v>
+      </c>
+      <c r="JL52" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JM52" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JN52" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="53" ht="13.9" customHeight="1" s="3">
@@ -43757,8 +44225,17 @@
       <c r="JJ53" s="2" t="n">
         <v>61</v>
       </c>
-      <c r="JK53" t="n">
+      <c r="JK53" s="2" t="n">
         <v>62</v>
+      </c>
+      <c r="JL53" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="JM53" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="JN53" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="54" ht="13.9" customHeight="1" s="3">
@@ -44574,7 +45051,16 @@
       <c r="JJ54" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JK54" t="n">
+      <c r="JK54" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="JL54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JM54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JN54" t="n">
         <v>4</v>
       </c>
     </row>
@@ -45391,8 +45877,17 @@
       <c r="JJ55" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="JK55" t="n">
+      <c r="JK55" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="JL55" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JM55" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JN55" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="56" ht="13.9" customHeight="1" s="3">
@@ -46208,8 +46703,17 @@
       <c r="JJ56" s="2" t="n">
         <v>66.7</v>
       </c>
-      <c r="JK56" t="n">
+      <c r="JK56" s="2" t="n">
         <v>87.5</v>
+      </c>
+      <c r="JL56" s="2" t="n">
+        <v>56.2</v>
+      </c>
+      <c r="JM56" s="2" t="n">
+        <v>56.2</v>
+      </c>
+      <c r="JN56" t="n">
+        <v>57.1</v>
       </c>
     </row>
     <row r="57" ht="13.9" customHeight="1" s="3">
@@ -47025,8 +47529,17 @@
       <c r="JJ57" s="2" t="n">
         <v>218</v>
       </c>
-      <c r="JK57" t="n">
+      <c r="JK57" s="2" t="n">
         <v>216</v>
+      </c>
+      <c r="JL57" s="2" t="n">
+        <v>216</v>
+      </c>
+      <c r="JM57" s="2" t="n">
+        <v>216</v>
+      </c>
+      <c r="JN57" t="n">
+        <v>213</v>
       </c>
     </row>
     <row r="58" ht="13.9" customHeight="1" s="3">
@@ -47842,8 +48355,17 @@
       <c r="JJ58" s="2" t="n">
         <v>109</v>
       </c>
-      <c r="JK58" t="n">
+      <c r="JK58" s="2" t="n">
         <v>119</v>
+      </c>
+      <c r="JL58" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="JM58" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="JN58" t="n">
+        <v>103</v>
       </c>
     </row>
     <row r="59" ht="13.9" customHeight="1" s="3">
@@ -48659,8 +49181,17 @@
       <c r="JJ59" s="2" t="n">
         <v>327</v>
       </c>
-      <c r="JK59" t="n">
+      <c r="JK59" s="2" t="n">
         <v>335</v>
+      </c>
+      <c r="JL59" s="2" t="n">
+        <v>320</v>
+      </c>
+      <c r="JM59" s="2" t="n">
+        <v>320</v>
+      </c>
+      <c r="JN59" t="n">
+        <v>316</v>
       </c>
     </row>
     <row r="60" ht="13.9" customHeight="1" s="3">
@@ -49476,8 +50007,17 @@
       <c r="JJ60" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="JK60" t="n">
+      <c r="JK60" s="2" t="n">
         <v>1.82</v>
+      </c>
+      <c r="JL60" s="2" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="JM60" s="2" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="JN60" t="n">
+        <v>2.07</v>
       </c>
     </row>
     <row r="61" ht="13.9" customHeight="1" s="3">
@@ -50293,8 +50833,17 @@
       <c r="JJ61" s="2" t="n">
         <v>98</v>
       </c>
-      <c r="JK61" t="n">
+      <c r="JK61" s="2" t="n">
         <v>97</v>
+      </c>
+      <c r="JL61" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="JM61" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="JN61" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="62" ht="13.9" customHeight="1" s="3">
@@ -51110,8 +51659,17 @@
       <c r="JJ62" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="JK62" t="n">
+      <c r="JK62" s="2" t="n">
         <v>53</v>
+      </c>
+      <c r="JL62" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="JM62" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="JN62" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="63" ht="13.9" customHeight="1" s="3">
@@ -51927,8 +52485,17 @@
       <c r="JJ63" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="JK63" t="n">
+      <c r="JK63" s="2" t="n">
         <v>43</v>
+      </c>
+      <c r="JL63" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JM63" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JN63" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="64" ht="13.9" customHeight="1" s="3">
@@ -52744,8 +53311,17 @@
       <c r="JJ64" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="JK64" t="n">
+      <c r="JK64" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="JL64" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="JM64" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="JN64" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="65" ht="13.9" customHeight="1" s="3">
@@ -53561,8 +54137,17 @@
       <c r="JJ65" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="JK65" t="n">
+      <c r="JK65" s="2" t="n">
         <v>16</v>
+      </c>
+      <c r="JL65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JM65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JN65" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="66" ht="13.9" customHeight="1" s="3">
@@ -54378,8 +54963,17 @@
       <c r="JJ66" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="JK66" t="n">
+      <c r="JK66" s="2" t="n">
         <v>18</v>
+      </c>
+      <c r="JL66" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="JM66" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="JN66" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="67" ht="13.9" customHeight="1" s="3">
@@ -55195,8 +55789,17 @@
       <c r="JJ67" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JK67" t="n">
+      <c r="JK67" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="JL67" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JM67" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JN67" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="68" ht="13.9" customHeight="1" s="3">
@@ -56012,8 +56615,17 @@
       <c r="JJ68" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="JK68" t="n">
+      <c r="JK68" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="JL68" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JM68" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JN68" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="69" ht="13.9" customHeight="1" s="3">
@@ -56829,8 +57441,17 @@
       <c r="JJ69" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="JK69" t="n">
+      <c r="JK69" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="JL69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JM69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JN69" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="70" ht="13.9" customHeight="1" s="3">
@@ -57646,8 +58267,17 @@
       <c r="JJ70" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="JK70" t="n">
+      <c r="JK70" s="2" t="n">
         <v>25</v>
+      </c>
+      <c r="JL70" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="JM70" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="JN70" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="71" ht="13.9" customHeight="1" s="3">
@@ -58463,8 +59093,17 @@
       <c r="JJ71" s="2" t="n">
         <v>42.9</v>
       </c>
-      <c r="JK71" t="n">
+      <c r="JK71" s="2" t="n">
         <v>72</v>
+      </c>
+      <c r="JL71" s="2" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="JM71" s="2" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="JN71" t="n">
+        <v>45.8</v>
       </c>
     </row>
     <row r="72" ht="13.9" customHeight="1" s="3">
@@ -59280,8 +59919,17 @@
       <c r="JJ72" s="2" t="n">
         <v>36.33</v>
       </c>
-      <c r="JK72" t="n">
+      <c r="JK72" s="2" t="n">
         <v>18.61</v>
+      </c>
+      <c r="JL72" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="JM72" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="JN72" t="n">
+        <v>28.73</v>
       </c>
     </row>
     <row r="73" ht="13.9" customHeight="1" s="3">
@@ -60097,8 +60745,17 @@
       <c r="JJ73" s="2" t="n">
         <v>15.57</v>
       </c>
-      <c r="JK73" t="n">
+      <c r="JK73" s="2" t="n">
         <v>13.4</v>
+      </c>
+      <c r="JL73" s="2" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="JM73" s="2" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="JN73" t="n">
+        <v>13.17</v>
       </c>
     </row>
     <row r="74" ht="13.9" customHeight="1" s="3">
@@ -60914,8 +61571,17 @@
       <c r="JJ74" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="JK74" t="n">
+      <c r="JK74" s="2" t="n">
         <v>40</v>
+      </c>
+      <c r="JL74" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="JM74" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="JN74" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="75" ht="13.9" customHeight="1" s="3">
@@ -61731,8 +62397,17 @@
       <c r="JJ75" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="JK75" t="n">
+      <c r="JK75" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="JL75" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="JM75" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="JN75" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="76" ht="13.9" customHeight="1" s="3">
@@ -62548,8 +63223,17 @@
       <c r="JJ76" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="JK76" t="n">
+      <c r="JK76" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="JL76" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="JM76" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="JN76" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="77" ht="13.9" customHeight="1" s="3">
@@ -63365,8 +64049,17 @@
       <c r="JJ77" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="JK77" t="n">
+      <c r="JK77" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="JL77" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="JM77" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="JN77" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="78" ht="13.9" customHeight="1" s="3">
@@ -64182,8 +64875,17 @@
       <c r="JJ78" s="2" t="n">
         <v>2.38</v>
       </c>
-      <c r="JK78" t="n">
+      <c r="JK78" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="JL78" s="2" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="JM78" s="2" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="JN78" t="n">
+        <v>2.29</v>
       </c>
     </row>
     <row r="79" ht="13.9" customHeight="1" s="3">
@@ -64999,8 +65701,17 @@
       <c r="JJ79" s="2" t="n">
         <v>5.56</v>
       </c>
-      <c r="JK79" t="n">
+      <c r="JK79" s="2" t="n">
         <v>2.78</v>
+      </c>
+      <c r="JL79" s="2" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="JM79" s="2" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="JN79" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="80" ht="13.9" customHeight="1" s="3">
@@ -65816,8 +66527,17 @@
       <c r="JJ80" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="JK80" t="n">
+      <c r="JK80" s="2" t="n">
         <v>46</v>
+      </c>
+      <c r="JL80" s="2" t="n">
+        <v>34.9</v>
+      </c>
+      <c r="JM80" s="2" t="n">
+        <v>34.9</v>
+      </c>
+      <c r="JN80" t="n">
+        <v>38.2</v>
       </c>
     </row>
     <row r="81" ht="13.9" customHeight="1" s="3">
@@ -66633,8 +67353,17 @@
       <c r="JJ81" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="JK81" t="n">
+      <c r="JK81" s="2" t="n">
         <v>36</v>
+      </c>
+      <c r="JL81" s="2" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="JM81" s="2" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="JN81" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="82" ht="13.9" customHeight="1" s="3">
@@ -67450,8 +68179,17 @@
       <c r="JJ82" s="2" t="n">
         <v>188.3</v>
       </c>
-      <c r="JK82" t="n">
+      <c r="JK82" s="2" t="n">
         <v>187.2</v>
+      </c>
+      <c r="JL82" s="2" t="n">
+        <v>186.7</v>
+      </c>
+      <c r="JM82" s="2" t="n">
+        <v>186.7</v>
+      </c>
+      <c r="JN82" t="n">
+        <v>187.7</v>
       </c>
     </row>
     <row r="83" ht="13.9" customHeight="1" s="3">
@@ -68267,8 +69005,17 @@
       <c r="JJ83" s="2" t="n">
         <v>85.5</v>
       </c>
-      <c r="JK83" t="n">
+      <c r="JK83" s="2" t="n">
         <v>87.09999999999999</v>
+      </c>
+      <c r="JL83" s="2" t="n">
+        <v>86.09999999999999</v>
+      </c>
+      <c r="JM83" s="2" t="n">
+        <v>86.09999999999999</v>
+      </c>
+      <c r="JN83" t="n">
+        <v>88</v>
       </c>
     </row>
     <row r="84" ht="13.9" customHeight="1" s="3">
@@ -69084,8 +69831,17 @@
       <c r="JJ84" s="2" t="n">
         <v>25.49</v>
       </c>
-      <c r="JK84" t="n">
+      <c r="JK84" s="2" t="n">
         <v>25.8</v>
+      </c>
+      <c r="JL84" s="2" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="JM84" s="2" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="JN84" t="n">
+        <v>26.33</v>
       </c>
     </row>
     <row r="85" ht="13.9" customHeight="1" s="3">
@@ -69901,8 +70657,17 @@
       <c r="JJ85" s="2" t="n">
         <v>91.7</v>
       </c>
-      <c r="JK85" t="n">
+      <c r="JK85" s="2" t="n">
         <v>116.6</v>
+      </c>
+      <c r="JL85" s="2" t="n">
+        <v>131.5</v>
+      </c>
+      <c r="JM85" s="2" t="n">
+        <v>131.5</v>
+      </c>
+      <c r="JN85" t="n">
+        <v>122.7</v>
       </c>
     </row>
     <row r="86" ht="13.9" customHeight="1" s="3">
@@ -70718,8 +71483,17 @@
       <c r="JJ86" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JK86" t="n">
+      <c r="JK86" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="JL86" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JM86" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JN86" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="87" ht="13.9" customHeight="1" s="3">
@@ -71535,8 +72309,17 @@
       <c r="JJ87" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="JK87" t="n">
+      <c r="JK87" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="JL87" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="JM87" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="JN87" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="88" ht="13.9" customHeight="1" s="3">
@@ -72352,7 +73135,16 @@
       <c r="JJ88" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JK88" t="n">
+      <c r="JK88" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JL88" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JM88" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JN88" t="n">
         <v>9</v>
       </c>
     </row>
@@ -73169,8 +73961,17 @@
       <c r="JJ89" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="JK89" t="n">
+      <c r="JK89" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="JL89" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JM89" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JN89" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="90" ht="13.9" customHeight="1" s="3">
@@ -73986,8 +74787,17 @@
       <c r="JJ90" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="JK90" t="n">
+      <c r="JK90" s="2" t="n">
         <v>140</v>
+      </c>
+      <c r="JL90" s="2" t="n">
+        <v>144</v>
+      </c>
+      <c r="JM90" s="2" t="n">
+        <v>144</v>
+      </c>
+      <c r="JN90" t="n">
+        <v>156</v>
       </c>
     </row>
     <row r="91" ht="13.9" customHeight="1" s="3">
@@ -74803,8 +75613,17 @@
       <c r="JJ91" s="2" t="n">
         <v>193</v>
       </c>
-      <c r="JK91" t="n">
+      <c r="JK91" s="2" t="n">
         <v>202</v>
+      </c>
+      <c r="JL91" s="2" t="n">
+        <v>162</v>
+      </c>
+      <c r="JM91" s="2" t="n">
+        <v>162</v>
+      </c>
+      <c r="JN91" t="n">
+        <v>157</v>
       </c>
     </row>
     <row r="92" ht="13.9" customHeight="1" s="3">
@@ -75620,8 +76439,17 @@
       <c r="JJ92" s="2" t="n">
         <v>230</v>
       </c>
-      <c r="JK92" t="n">
+      <c r="JK92" s="2" t="n">
         <v>249</v>
+      </c>
+      <c r="JL92" s="2" t="n">
+        <v>212</v>
+      </c>
+      <c r="JM92" s="2" t="n">
+        <v>212</v>
+      </c>
+      <c r="JN92" t="n">
+        <v>208</v>
       </c>
     </row>
     <row r="93" ht="13.9" customHeight="1" s="3">
@@ -76437,8 +77265,17 @@
       <c r="JJ93" s="2" t="n">
         <v>70.3</v>
       </c>
-      <c r="JK93" t="n">
+      <c r="JK93" s="2" t="n">
         <v>74.3</v>
+      </c>
+      <c r="JL93" s="2" t="n">
+        <v>66.2</v>
+      </c>
+      <c r="JM93" s="2" t="n">
+        <v>66.2</v>
+      </c>
+      <c r="JN93" t="n">
+        <v>65.8</v>
       </c>
     </row>
     <row r="94" ht="13.9" customHeight="1" s="3">
@@ -77254,8 +78091,17 @@
       <c r="JJ94" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="JK94" t="n">
+      <c r="JK94" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="JL94" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="JM94" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="JN94" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="95" ht="13.9" customHeight="1" s="3">
@@ -78071,8 +78917,17 @@
       <c r="JJ95" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="JK95" t="n">
+      <c r="JK95" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="JL95" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="JM95" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="JN95" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="96" ht="13.9" customHeight="1" s="3">
@@ -78888,8 +79743,17 @@
       <c r="JJ96" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="JK96" t="n">
+      <c r="JK96" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="JL96" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="JM96" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="JN96" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="97" ht="13.9" customHeight="1" s="3">
@@ -79705,8 +80569,17 @@
       <c r="JJ97" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="JK97" t="n">
+      <c r="JK97" s="2" t="n">
         <v>40</v>
+      </c>
+      <c r="JL97" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="JM97" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="JN97" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="98" ht="13.9" customHeight="1" s="3">
@@ -80522,8 +81395,17 @@
       <c r="JJ98" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="JK98" t="n">
+      <c r="JK98" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="JL98" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="JM98" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="JN98" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="99" ht="13.9" customHeight="1" s="3">
@@ -81339,8 +82221,17 @@
       <c r="JJ99" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="JK99" t="n">
+      <c r="JK99" s="2" t="n">
         <v>48</v>
+      </c>
+      <c r="JL99" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JM99" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JN99" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="100" ht="13.9" customHeight="1" s="3">
@@ -82156,8 +83047,17 @@
       <c r="JJ100" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="JK100" t="n">
+      <c r="JK100" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="JL100" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JM100" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JN100" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="101" ht="13.9" customHeight="1" s="3">
@@ -82973,8 +83873,17 @@
       <c r="JJ101" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JK101" t="n">
+      <c r="JK101" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="JL101" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JM101" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JN101" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="102" ht="13.9" customHeight="1" s="3">
@@ -83790,8 +84699,17 @@
       <c r="JJ102" s="2" t="n">
         <v>77.8</v>
       </c>
-      <c r="JK102" t="n">
+      <c r="JK102" s="2" t="n">
         <v>72.2</v>
+      </c>
+      <c r="JL102" s="2" t="n">
+        <v>81.2</v>
+      </c>
+      <c r="JM102" s="2" t="n">
+        <v>81.2</v>
+      </c>
+      <c r="JN102" t="n">
+        <v>45.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made the predict into one big python script to be called from command line
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Brisbane_stats.xlsx
+++ b/django_AFL_ML/Data/Brisbane_stats.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JN102"/>
+  <dimension ref="A1:JP102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="HZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="IL36" activeCellId="0" sqref="IL36"/>
@@ -1282,7 +1282,13 @@
       <c r="JM1" s="2" t="n">
         <v>10742</v>
       </c>
-      <c r="JN1" t="n">
+      <c r="JN1" s="2" t="n">
+        <v>10746</v>
+      </c>
+      <c r="JO1" s="2" t="n">
+        <v>10746</v>
+      </c>
+      <c r="JP1" t="n">
         <v>10746</v>
       </c>
     </row>
@@ -2108,7 +2114,13 @@
       <c r="JM2" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="JN2" t="n">
+      <c r="JN2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JO2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JP2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2934,7 +2946,13 @@
       <c r="JM3" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="JN3" t="n">
+      <c r="JN3" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="JO3" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="JP3" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3760,7 +3778,13 @@
       <c r="JM4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="JN4" t="n">
+      <c r="JN4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JO4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JP4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4586,7 +4610,13 @@
       <c r="JM5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="JN5" t="n">
+      <c r="JN5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JO5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JP5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5412,7 +5442,13 @@
       <c r="JM6" s="2" t="n">
         <v>106</v>
       </c>
-      <c r="JN6" t="n">
+      <c r="JN6" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="JO6" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="JP6" t="n">
         <v>92</v>
       </c>
     </row>
@@ -6238,7 +6274,13 @@
       <c r="JM7" s="2" t="n">
         <v>104</v>
       </c>
-      <c r="JN7" t="n">
+      <c r="JN7" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="JO7" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="JP7" t="n">
         <v>79</v>
       </c>
     </row>
@@ -7064,7 +7106,13 @@
       <c r="JM8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="JN8" t="n">
+      <c r="JN8" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JO8" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JP8" t="n">
         <v>13</v>
       </c>
     </row>
@@ -7890,7 +7938,13 @@
       <c r="JM9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="JN9" t="n">
+      <c r="JN9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JO9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JP9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8716,7 +8770,13 @@
       <c r="JM10" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="JN10" t="n">
+      <c r="JN10" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JO10" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JP10" t="n">
         <v>11</v>
       </c>
     </row>
@@ -9542,7 +9602,13 @@
       <c r="JM11" s="2" t="n">
         <v>210</v>
       </c>
-      <c r="JN11" t="n">
+      <c r="JN11" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JO11" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JP11" t="n">
         <v>229</v>
       </c>
     </row>
@@ -10368,7 +10434,13 @@
       <c r="JM12" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="JN12" t="n">
+      <c r="JN12" s="2" t="n">
+        <v>111</v>
+      </c>
+      <c r="JO12" s="2" t="n">
+        <v>111</v>
+      </c>
+      <c r="JP12" t="n">
         <v>111</v>
       </c>
     </row>
@@ -11194,7 +11266,13 @@
       <c r="JM13" s="2" t="n">
         <v>336</v>
       </c>
-      <c r="JN13" t="n">
+      <c r="JN13" s="2" t="n">
+        <v>340</v>
+      </c>
+      <c r="JO13" s="2" t="n">
+        <v>340</v>
+      </c>
+      <c r="JP13" t="n">
         <v>340</v>
       </c>
     </row>
@@ -12020,7 +12098,13 @@
       <c r="JM14" s="2" t="n">
         <v>1.67</v>
       </c>
-      <c r="JN14" t="n">
+      <c r="JN14" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="JO14" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="JP14" t="n">
         <v>2.06</v>
       </c>
     </row>
@@ -12846,7 +12930,13 @@
       <c r="JM15" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="JN15" t="n">
+      <c r="JN15" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="JO15" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="JP15" t="n">
         <v>92</v>
       </c>
     </row>
@@ -13672,7 +13762,13 @@
       <c r="JM16" s="2" t="n">
         <v>56</v>
       </c>
-      <c r="JN16" t="n">
+      <c r="JN16" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="JO16" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="JP16" t="n">
         <v>74</v>
       </c>
     </row>
@@ -14498,7 +14594,13 @@
       <c r="JM17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="JN17" t="n">
+      <c r="JN17" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="JO17" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="JP17" t="n">
         <v>33</v>
       </c>
     </row>
@@ -15324,7 +15426,13 @@
       <c r="JM18" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="JN18" t="n">
+      <c r="JN18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JO18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JP18" t="n">
         <v>22</v>
       </c>
     </row>
@@ -16150,7 +16258,13 @@
       <c r="JM19" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="JN19" t="n">
+      <c r="JN19" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="JO19" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="JP19" t="n">
         <v>19</v>
       </c>
     </row>
@@ -16976,7 +17090,13 @@
       <c r="JM20" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="JN20" t="n">
+      <c r="JN20" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="JO20" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="JP20" t="n">
         <v>14</v>
       </c>
     </row>
@@ -17802,7 +17922,13 @@
       <c r="JM21" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="JN21" t="n">
+      <c r="JN21" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JO21" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JP21" t="n">
         <v>8</v>
       </c>
     </row>
@@ -18628,7 +18754,13 @@
       <c r="JM22" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JN22" t="n">
+      <c r="JN22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JO22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JP22" t="n">
         <v>7</v>
       </c>
     </row>
@@ -19454,7 +19586,13 @@
       <c r="JM23" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="JN23" t="n">
+      <c r="JN23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JO23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JP23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -20280,7 +20418,13 @@
       <c r="JM24" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="JN24" t="n">
+      <c r="JN24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JO24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JP24" t="n">
         <v>22</v>
       </c>
     </row>
@@ -21106,7 +21250,13 @@
       <c r="JM25" s="2" t="n">
         <v>61.5</v>
       </c>
-      <c r="JN25" t="n">
+      <c r="JN25" s="2" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="JO25" s="2" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="JP25" t="n">
         <v>63.6</v>
       </c>
     </row>
@@ -21932,7 +22082,13 @@
       <c r="JM26" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="JN26" t="n">
+      <c r="JN26" s="2" t="n">
+        <v>24.29</v>
+      </c>
+      <c r="JO26" s="2" t="n">
+        <v>24.29</v>
+      </c>
+      <c r="JP26" t="n">
         <v>24.29</v>
       </c>
     </row>
@@ -22758,7 +22914,13 @@
       <c r="JM27" s="2" t="n">
         <v>12.92</v>
       </c>
-      <c r="JN27" t="n">
+      <c r="JN27" s="2" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="JO27" s="2" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="JP27" t="n">
         <v>15.45</v>
       </c>
     </row>
@@ -23584,7 +23746,13 @@
       <c r="JM28" s="2" t="n">
         <v>47</v>
       </c>
-      <c r="JN28" t="n">
+      <c r="JN28" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="JO28" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="JP28" t="n">
         <v>37</v>
       </c>
     </row>
@@ -24410,7 +24578,13 @@
       <c r="JM29" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="JN29" t="n">
+      <c r="JN29" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JO29" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JP29" t="n">
         <v>55</v>
       </c>
     </row>
@@ -25236,7 +25410,13 @@
       <c r="JM30" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="JN30" t="n">
+      <c r="JN30" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JO30" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JP30" t="n">
         <v>44</v>
       </c>
     </row>
@@ -26062,7 +26242,13 @@
       <c r="JM31" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="JN31" t="n">
+      <c r="JN31" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="JO31" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="JP31" t="n">
         <v>53</v>
       </c>
     </row>
@@ -26888,7 +27074,13 @@
       <c r="JM32" s="2" t="n">
         <v>2.27</v>
       </c>
-      <c r="JN32" t="n">
+      <c r="JN32" s="2" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="JO32" s="2" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="JP32" t="n">
         <v>2.41</v>
       </c>
     </row>
@@ -27714,7 +27906,13 @@
       <c r="JM33" s="2" t="n">
         <v>3.69</v>
       </c>
-      <c r="JN33" t="n">
+      <c r="JN33" s="2" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="JO33" s="2" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="JP33" t="n">
         <v>3.79</v>
       </c>
     </row>
@@ -28540,7 +28738,13 @@
       <c r="JM34" s="2" t="n">
         <v>39</v>
       </c>
-      <c r="JN34" t="n">
+      <c r="JN34" s="2" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="JO34" s="2" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="JP34" t="n">
         <v>39.6</v>
       </c>
     </row>
@@ -29366,7 +29570,13 @@
       <c r="JM35" s="2" t="n">
         <v>27.1</v>
       </c>
-      <c r="JN35" t="n">
+      <c r="JN35" s="2" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="JO35" s="2" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="JP35" t="n">
         <v>26.4</v>
       </c>
     </row>
@@ -30192,7 +30402,13 @@
       <c r="JM36" s="2" t="n">
         <v>188.1</v>
       </c>
-      <c r="JN36" t="n">
+      <c r="JN36" s="2" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="JO36" s="2" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="JP36" t="n">
         <v>187.9</v>
       </c>
     </row>
@@ -31018,7 +31234,13 @@
       <c r="JM37" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="JN37" t="n">
+      <c r="JN37" s="2" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="JO37" s="2" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="JP37" t="n">
         <v>87.3</v>
       </c>
     </row>
@@ -31844,7 +32066,13 @@
       <c r="JM38" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="JN38" t="n">
+      <c r="JN38" s="2" t="n">
+        <v>25.49</v>
+      </c>
+      <c r="JO38" s="2" t="n">
+        <v>25.49</v>
+      </c>
+      <c r="JP38" t="n">
         <v>25.49</v>
       </c>
     </row>
@@ -32670,7 +32898,13 @@
       <c r="JM39" s="2" t="n">
         <v>120.9</v>
       </c>
-      <c r="JN39" t="n">
+      <c r="JN39" s="2" t="n">
+        <v>106.7</v>
+      </c>
+      <c r="JO39" s="2" t="n">
+        <v>106.7</v>
+      </c>
+      <c r="JP39" t="n">
         <v>106.7</v>
       </c>
     </row>
@@ -33496,7 +33730,13 @@
       <c r="JM40" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JN40" t="n">
+      <c r="JN40" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JO40" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JP40" t="n">
         <v>6</v>
       </c>
     </row>
@@ -34322,7 +34562,13 @@
       <c r="JM41" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="JN41" t="n">
+      <c r="JN41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JO41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JP41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -35148,7 +35394,13 @@
       <c r="JM42" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JN42" t="n">
+      <c r="JN42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JO42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JP42" t="n">
         <v>5</v>
       </c>
     </row>
@@ -35974,7 +36226,13 @@
       <c r="JM43" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="JN43" t="n">
+      <c r="JN43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JO43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JP43" t="n">
         <v>7</v>
       </c>
     </row>
@@ -36800,7 +37058,13 @@
       <c r="JM44" s="2" t="n">
         <v>149</v>
       </c>
-      <c r="JN44" t="n">
+      <c r="JN44" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="JO44" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="JP44" t="n">
         <v>137</v>
       </c>
     </row>
@@ -37626,7 +37890,13 @@
       <c r="JM45" s="2" t="n">
         <v>182</v>
       </c>
-      <c r="JN45" t="n">
+      <c r="JN45" s="2" t="n">
+        <v>194</v>
+      </c>
+      <c r="JO45" s="2" t="n">
+        <v>194</v>
+      </c>
+      <c r="JP45" t="n">
         <v>194</v>
       </c>
     </row>
@@ -38452,7 +38722,13 @@
       <c r="JM46" s="2" t="n">
         <v>229</v>
       </c>
-      <c r="JN46" t="n">
+      <c r="JN46" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JO46" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JP46" t="n">
         <v>229</v>
       </c>
     </row>
@@ -39278,7 +39554,13 @@
       <c r="JM47" s="2" t="n">
         <v>68.2</v>
       </c>
-      <c r="JN47" t="n">
+      <c r="JN47" s="2" t="n">
+        <v>67.40000000000001</v>
+      </c>
+      <c r="JO47" s="2" t="n">
+        <v>67.40000000000001</v>
+      </c>
+      <c r="JP47" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -40104,7 +40386,13 @@
       <c r="JM48" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="JN48" t="n">
+      <c r="JN48" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JO48" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JP48" t="n">
         <v>55</v>
       </c>
     </row>
@@ -40930,7 +41218,13 @@
       <c r="JM49" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JN49" t="n">
+      <c r="JN49" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JO49" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JP49" t="n">
         <v>7</v>
       </c>
     </row>
@@ -41756,7 +42050,13 @@
       <c r="JM50" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="JN50" t="n">
+      <c r="JN50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JO50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JP50" t="n">
         <v>8</v>
       </c>
     </row>
@@ -42582,7 +42882,13 @@
       <c r="JM51" s="2" t="n">
         <v>47</v>
       </c>
-      <c r="JN51" t="n">
+      <c r="JN51" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="JO51" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="JP51" t="n">
         <v>37</v>
       </c>
     </row>
@@ -43408,7 +43714,13 @@
       <c r="JM52" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="JN52" t="n">
+      <c r="JN52" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JO52" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JP52" t="n">
         <v>44</v>
       </c>
     </row>
@@ -44234,7 +44546,13 @@
       <c r="JM53" s="2" t="n">
         <v>53</v>
       </c>
-      <c r="JN53" t="n">
+      <c r="JN53" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="JO53" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="JP53" t="n">
         <v>70</v>
       </c>
     </row>
@@ -45060,7 +45378,13 @@
       <c r="JM54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="JN54" t="n">
+      <c r="JN54" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="JO54" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="JP54" t="n">
         <v>4</v>
       </c>
     </row>
@@ -45886,7 +46210,13 @@
       <c r="JM55" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="JN55" t="n">
+      <c r="JN55" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JO55" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JP55" t="n">
         <v>8</v>
       </c>
     </row>
@@ -46712,7 +47042,13 @@
       <c r="JM56" s="2" t="n">
         <v>56.2</v>
       </c>
-      <c r="JN56" t="n">
+      <c r="JN56" s="2" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="JO56" s="2" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="JP56" t="n">
         <v>57.1</v>
       </c>
     </row>
@@ -47538,7 +47874,13 @@
       <c r="JM57" s="2" t="n">
         <v>216</v>
       </c>
-      <c r="JN57" t="n">
+      <c r="JN57" s="2" t="n">
+        <v>213</v>
+      </c>
+      <c r="JO57" s="2" t="n">
+        <v>213</v>
+      </c>
+      <c r="JP57" t="n">
         <v>213</v>
       </c>
     </row>
@@ -48364,7 +48706,13 @@
       <c r="JM58" s="2" t="n">
         <v>104</v>
       </c>
-      <c r="JN58" t="n">
+      <c r="JN58" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="JO58" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="JP58" t="n">
         <v>103</v>
       </c>
     </row>
@@ -49190,7 +49538,13 @@
       <c r="JM59" s="2" t="n">
         <v>320</v>
       </c>
-      <c r="JN59" t="n">
+      <c r="JN59" s="2" t="n">
+        <v>316</v>
+      </c>
+      <c r="JO59" s="2" t="n">
+        <v>316</v>
+      </c>
+      <c r="JP59" t="n">
         <v>316</v>
       </c>
     </row>
@@ -50016,7 +50370,13 @@
       <c r="JM60" s="2" t="n">
         <v>2.08</v>
       </c>
-      <c r="JN60" t="n">
+      <c r="JN60" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="JO60" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="JP60" t="n">
         <v>2.07</v>
       </c>
     </row>
@@ -50842,7 +51202,13 @@
       <c r="JM61" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="JN61" t="n">
+      <c r="JN61" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="JO61" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="JP61" t="n">
         <v>78</v>
       </c>
     </row>
@@ -51668,7 +52034,13 @@
       <c r="JM62" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="JN62" t="n">
+      <c r="JN62" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="JO62" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="JP62" t="n">
         <v>73</v>
       </c>
     </row>
@@ -52494,7 +52866,13 @@
       <c r="JM63" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="JN63" t="n">
+      <c r="JN63" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="JO63" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="JP63" t="n">
         <v>48</v>
       </c>
     </row>
@@ -53320,7 +53698,13 @@
       <c r="JM64" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="JN64" t="n">
+      <c r="JN64" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="JO64" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="JP64" t="n">
         <v>19</v>
       </c>
     </row>
@@ -54146,7 +54530,13 @@
       <c r="JM65" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="JN65" t="n">
+      <c r="JN65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JO65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JP65" t="n">
         <v>22</v>
       </c>
     </row>
@@ -54972,7 +55362,13 @@
       <c r="JM66" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="JN66" t="n">
+      <c r="JN66" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JO66" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JP66" t="n">
         <v>11</v>
       </c>
     </row>
@@ -55798,7 +56194,13 @@
       <c r="JM67" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="JN67" t="n">
+      <c r="JN67" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JO67" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JP67" t="n">
         <v>5</v>
       </c>
     </row>
@@ -56624,7 +57026,13 @@
       <c r="JM68" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JN68" t="n">
+      <c r="JN68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JO68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JP68" t="n">
         <v>10</v>
       </c>
     </row>
@@ -57450,7 +57858,13 @@
       <c r="JM69" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="JN69" t="n">
+      <c r="JN69" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JO69" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JP69" t="n">
         <v>3</v>
       </c>
     </row>
@@ -58276,7 +58690,13 @@
       <c r="JM70" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="JN70" t="n">
+      <c r="JN70" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="JO70" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="JP70" t="n">
         <v>24</v>
       </c>
     </row>
@@ -59102,7 +59522,13 @@
       <c r="JM71" s="2" t="n">
         <v>66.7</v>
       </c>
-      <c r="JN71" t="n">
+      <c r="JN71" s="2" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="JO71" s="2" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="JP71" t="n">
         <v>45.8</v>
       </c>
     </row>
@@ -59928,7 +60354,13 @@
       <c r="JM72" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="JN72" t="n">
+      <c r="JN72" s="2" t="n">
+        <v>28.73</v>
+      </c>
+      <c r="JO72" s="2" t="n">
+        <v>28.73</v>
+      </c>
+      <c r="JP72" t="n">
         <v>28.73</v>
       </c>
     </row>
@@ -60754,7 +61186,13 @@
       <c r="JM73" s="2" t="n">
         <v>13.33</v>
       </c>
-      <c r="JN73" t="n">
+      <c r="JN73" s="2" t="n">
+        <v>13.17</v>
+      </c>
+      <c r="JO73" s="2" t="n">
+        <v>13.17</v>
+      </c>
+      <c r="JP73" t="n">
         <v>13.17</v>
       </c>
     </row>
@@ -61580,7 +62018,13 @@
       <c r="JM74" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="JN74" t="n">
+      <c r="JN74" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JO74" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JP74" t="n">
         <v>51</v>
       </c>
     </row>
@@ -62406,7 +62850,13 @@
       <c r="JM75" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="JN75" t="n">
+      <c r="JN75" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JO75" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JP75" t="n">
         <v>58</v>
       </c>
     </row>
@@ -63232,7 +63682,13 @@
       <c r="JM76" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="JN76" t="n">
+      <c r="JN76" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JO76" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JP76" t="n">
         <v>39</v>
       </c>
     </row>
@@ -64058,7 +64514,13 @@
       <c r="JM77" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="JN77" t="n">
+      <c r="JN77" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JO77" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JP77" t="n">
         <v>55</v>
       </c>
     </row>
@@ -64884,7 +65346,13 @@
       <c r="JM78" s="2" t="n">
         <v>2.62</v>
       </c>
-      <c r="JN78" t="n">
+      <c r="JN78" s="2" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="JO78" s="2" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="JP78" t="n">
         <v>2.29</v>
       </c>
     </row>
@@ -65710,7 +66178,13 @@
       <c r="JM79" s="2" t="n">
         <v>3.94</v>
       </c>
-      <c r="JN79" t="n">
+      <c r="JN79" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JO79" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JP79" t="n">
         <v>5</v>
       </c>
     </row>
@@ -66536,7 +67010,13 @@
       <c r="JM80" s="2" t="n">
         <v>34.9</v>
       </c>
-      <c r="JN80" t="n">
+      <c r="JN80" s="2" t="n">
+        <v>38.2</v>
+      </c>
+      <c r="JO80" s="2" t="n">
+        <v>38.2</v>
+      </c>
+      <c r="JP80" t="n">
         <v>38.2</v>
       </c>
     </row>
@@ -67362,7 +67842,13 @@
       <c r="JM81" s="2" t="n">
         <v>25.4</v>
       </c>
-      <c r="JN81" t="n">
+      <c r="JN81" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="JO81" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="JP81" t="n">
         <v>20</v>
       </c>
     </row>
@@ -68188,7 +68674,13 @@
       <c r="JM82" s="2" t="n">
         <v>186.7</v>
       </c>
-      <c r="JN82" t="n">
+      <c r="JN82" s="2" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="JO82" s="2" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="JP82" t="n">
         <v>187.7</v>
       </c>
     </row>
@@ -69014,7 +69506,13 @@
       <c r="JM83" s="2" t="n">
         <v>86.09999999999999</v>
       </c>
-      <c r="JN83" t="n">
+      <c r="JN83" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="JO83" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="JP83" t="n">
         <v>88</v>
       </c>
     </row>
@@ -69840,7 +70338,13 @@
       <c r="JM84" s="2" t="n">
         <v>26.8</v>
       </c>
-      <c r="JN84" t="n">
+      <c r="JN84" s="2" t="n">
+        <v>26.33</v>
+      </c>
+      <c r="JO84" s="2" t="n">
+        <v>26.33</v>
+      </c>
+      <c r="JP84" t="n">
         <v>26.33</v>
       </c>
     </row>
@@ -70666,7 +71170,13 @@
       <c r="JM85" s="2" t="n">
         <v>131.5</v>
       </c>
-      <c r="JN85" t="n">
+      <c r="JN85" s="2" t="n">
+        <v>122.7</v>
+      </c>
+      <c r="JO85" s="2" t="n">
+        <v>122.7</v>
+      </c>
+      <c r="JP85" t="n">
         <v>122.7</v>
       </c>
     </row>
@@ -71492,7 +72002,13 @@
       <c r="JM86" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JN86" t="n">
+      <c r="JN86" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JO86" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JP86" t="n">
         <v>2</v>
       </c>
     </row>
@@ -72318,7 +72834,13 @@
       <c r="JM87" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="JN87" t="n">
+      <c r="JN87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JO87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JP87" t="n">
         <v>5</v>
       </c>
     </row>
@@ -73144,7 +73666,13 @@
       <c r="JM88" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JN88" t="n">
+      <c r="JN88" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JO88" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JP88" t="n">
         <v>9</v>
       </c>
     </row>
@@ -73970,7 +74498,13 @@
       <c r="JM89" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="JN89" t="n">
+      <c r="JN89" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JO89" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JP89" t="n">
         <v>7</v>
       </c>
     </row>
@@ -74796,7 +75330,13 @@
       <c r="JM90" s="2" t="n">
         <v>144</v>
       </c>
-      <c r="JN90" t="n">
+      <c r="JN90" s="2" t="n">
+        <v>156</v>
+      </c>
+      <c r="JO90" s="2" t="n">
+        <v>156</v>
+      </c>
+      <c r="JP90" t="n">
         <v>156</v>
       </c>
     </row>
@@ -75622,7 +76162,13 @@
       <c r="JM91" s="2" t="n">
         <v>162</v>
       </c>
-      <c r="JN91" t="n">
+      <c r="JN91" s="2" t="n">
+        <v>157</v>
+      </c>
+      <c r="JO91" s="2" t="n">
+        <v>157</v>
+      </c>
+      <c r="JP91" t="n">
         <v>157</v>
       </c>
     </row>
@@ -76448,7 +76994,13 @@
       <c r="JM92" s="2" t="n">
         <v>212</v>
       </c>
-      <c r="JN92" t="n">
+      <c r="JN92" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="JO92" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="JP92" t="n">
         <v>208</v>
       </c>
     </row>
@@ -77274,7 +77826,13 @@
       <c r="JM93" s="2" t="n">
         <v>66.2</v>
       </c>
-      <c r="JN93" t="n">
+      <c r="JN93" s="2" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="JO93" s="2" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="JP93" t="n">
         <v>65.8</v>
       </c>
     </row>
@@ -78100,7 +78658,13 @@
       <c r="JM94" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="JN94" t="n">
+      <c r="JN94" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JO94" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JP94" t="n">
         <v>58</v>
       </c>
     </row>
@@ -78926,7 +79490,13 @@
       <c r="JM95" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="JN95" t="n">
+      <c r="JN95" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JO95" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JP95" t="n">
         <v>13</v>
       </c>
     </row>
@@ -79752,7 +80322,13 @@
       <c r="JM96" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="JN96" t="n">
+      <c r="JN96" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JO96" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JP96" t="n">
         <v>10</v>
       </c>
     </row>
@@ -80578,7 +81154,13 @@
       <c r="JM97" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="JN97" t="n">
+      <c r="JN97" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JO97" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JP97" t="n">
         <v>51</v>
       </c>
     </row>
@@ -81404,7 +81986,13 @@
       <c r="JM98" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="JN98" t="n">
+      <c r="JN98" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JO98" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JP98" t="n">
         <v>39</v>
       </c>
     </row>
@@ -82230,7 +82818,13 @@
       <c r="JM99" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="JN99" t="n">
+      <c r="JN99" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JO99" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JP99" t="n">
         <v>44</v>
       </c>
     </row>
@@ -83056,7 +83650,13 @@
       <c r="JM100" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JN100" t="n">
+      <c r="JN100" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JO100" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JP100" t="n">
         <v>3</v>
       </c>
     </row>
@@ -83882,7 +84482,13 @@
       <c r="JM101" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="JN101" t="n">
+      <c r="JN101" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JO101" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JP101" t="n">
         <v>5</v>
       </c>
     </row>
@@ -84708,7 +85314,13 @@
       <c r="JM102" s="2" t="n">
         <v>81.2</v>
       </c>
-      <c r="JN102" t="n">
+      <c r="JN102" s="2" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="JO102" s="2" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="JP102" t="n">
         <v>45.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clean data fixes my finals round numbering mistake. predict now outputs to one singular prediction. Streamlined command line process.
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Brisbane_stats.xlsx
+++ b/django_AFL_ML/Data/Brisbane_stats.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JP102"/>
+  <dimension ref="A1:JS102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="HZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="IL36" activeCellId="0" sqref="IL36"/>
@@ -1288,7 +1288,16 @@
       <c r="JO1" s="2" t="n">
         <v>10746</v>
       </c>
-      <c r="JP1" t="n">
+      <c r="JP1" s="2" t="n">
+        <v>10746</v>
+      </c>
+      <c r="JQ1" s="2" t="n">
+        <v>10746</v>
+      </c>
+      <c r="JR1" s="2" t="n">
+        <v>10746</v>
+      </c>
+      <c r="JS1" t="n">
         <v>10746</v>
       </c>
     </row>
@@ -2120,7 +2129,16 @@
       <c r="JO2" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="JP2" t="n">
+      <c r="JP2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JQ2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JR2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JS2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2952,7 +2970,16 @@
       <c r="JO3" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="JP3" t="n">
+      <c r="JP3" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="JQ3" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="JR3" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="JS3" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3784,7 +3811,16 @@
       <c r="JO4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="JP4" t="n">
+      <c r="JP4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JQ4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JR4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JS4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4616,7 +4652,16 @@
       <c r="JO5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="JP5" t="n">
+      <c r="JP5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JQ5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JR5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JS5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5448,7 +5493,16 @@
       <c r="JO6" s="2" t="n">
         <v>92</v>
       </c>
-      <c r="JP6" t="n">
+      <c r="JP6" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="JQ6" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="JR6" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="JS6" t="n">
         <v>92</v>
       </c>
     </row>
@@ -6280,7 +6334,16 @@
       <c r="JO7" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="JP7" t="n">
+      <c r="JP7" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="JQ7" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="JR7" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="JS7" t="n">
         <v>79</v>
       </c>
     </row>
@@ -7112,7 +7175,16 @@
       <c r="JO8" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="JP8" t="n">
+      <c r="JP8" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JQ8" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JR8" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JS8" t="n">
         <v>13</v>
       </c>
     </row>
@@ -7944,7 +8016,16 @@
       <c r="JO9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="JP9" t="n">
+      <c r="JP9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JQ9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JR9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JS9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8776,7 +8857,16 @@
       <c r="JO10" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="JP10" t="n">
+      <c r="JP10" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JQ10" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JR10" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JS10" t="n">
         <v>11</v>
       </c>
     </row>
@@ -9608,7 +9698,16 @@
       <c r="JO11" s="2" t="n">
         <v>229</v>
       </c>
-      <c r="JP11" t="n">
+      <c r="JP11" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JQ11" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JR11" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JS11" t="n">
         <v>229</v>
       </c>
     </row>
@@ -10440,7 +10539,16 @@
       <c r="JO12" s="2" t="n">
         <v>111</v>
       </c>
-      <c r="JP12" t="n">
+      <c r="JP12" s="2" t="n">
+        <v>111</v>
+      </c>
+      <c r="JQ12" s="2" t="n">
+        <v>111</v>
+      </c>
+      <c r="JR12" s="2" t="n">
+        <v>111</v>
+      </c>
+      <c r="JS12" t="n">
         <v>111</v>
       </c>
     </row>
@@ -11272,7 +11380,16 @@
       <c r="JO13" s="2" t="n">
         <v>340</v>
       </c>
-      <c r="JP13" t="n">
+      <c r="JP13" s="2" t="n">
+        <v>340</v>
+      </c>
+      <c r="JQ13" s="2" t="n">
+        <v>340</v>
+      </c>
+      <c r="JR13" s="2" t="n">
+        <v>340</v>
+      </c>
+      <c r="JS13" t="n">
         <v>340</v>
       </c>
     </row>
@@ -12104,7 +12221,16 @@
       <c r="JO14" s="2" t="n">
         <v>2.06</v>
       </c>
-      <c r="JP14" t="n">
+      <c r="JP14" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="JQ14" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="JR14" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="JS14" t="n">
         <v>2.06</v>
       </c>
     </row>
@@ -12936,7 +13062,16 @@
       <c r="JO15" s="2" t="n">
         <v>92</v>
       </c>
-      <c r="JP15" t="n">
+      <c r="JP15" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="JQ15" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="JR15" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="JS15" t="n">
         <v>92</v>
       </c>
     </row>
@@ -13768,7 +13903,16 @@
       <c r="JO16" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="JP16" t="n">
+      <c r="JP16" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="JQ16" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="JR16" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="JS16" t="n">
         <v>74</v>
       </c>
     </row>
@@ -14600,7 +14744,16 @@
       <c r="JO17" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="JP17" t="n">
+      <c r="JP17" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="JQ17" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="JR17" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="JS17" t="n">
         <v>33</v>
       </c>
     </row>
@@ -15432,7 +15585,16 @@
       <c r="JO18" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="JP18" t="n">
+      <c r="JP18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JQ18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JR18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JS18" t="n">
         <v>22</v>
       </c>
     </row>
@@ -16264,7 +16426,16 @@
       <c r="JO19" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="JP19" t="n">
+      <c r="JP19" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="JQ19" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="JR19" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="JS19" t="n">
         <v>19</v>
       </c>
     </row>
@@ -17096,7 +17267,16 @@
       <c r="JO20" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="JP20" t="n">
+      <c r="JP20" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="JQ20" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="JR20" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="JS20" t="n">
         <v>14</v>
       </c>
     </row>
@@ -17928,7 +18108,16 @@
       <c r="JO21" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="JP21" t="n">
+      <c r="JP21" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JQ21" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JR21" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JS21" t="n">
         <v>8</v>
       </c>
     </row>
@@ -18760,7 +18949,16 @@
       <c r="JO22" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JP22" t="n">
+      <c r="JP22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JQ22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JR22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JS22" t="n">
         <v>7</v>
       </c>
     </row>
@@ -19592,7 +19790,16 @@
       <c r="JO23" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="JP23" t="n">
+      <c r="JP23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JQ23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JR23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JS23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -20424,7 +20631,16 @@
       <c r="JO24" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="JP24" t="n">
+      <c r="JP24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JQ24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JR24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JS24" t="n">
         <v>22</v>
       </c>
     </row>
@@ -21256,7 +21472,16 @@
       <c r="JO25" s="2" t="n">
         <v>63.6</v>
       </c>
-      <c r="JP25" t="n">
+      <c r="JP25" s="2" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="JQ25" s="2" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="JR25" s="2" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="JS25" t="n">
         <v>63.6</v>
       </c>
     </row>
@@ -22088,7 +22313,16 @@
       <c r="JO26" s="2" t="n">
         <v>24.29</v>
       </c>
-      <c r="JP26" t="n">
+      <c r="JP26" s="2" t="n">
+        <v>24.29</v>
+      </c>
+      <c r="JQ26" s="2" t="n">
+        <v>24.29</v>
+      </c>
+      <c r="JR26" s="2" t="n">
+        <v>24.29</v>
+      </c>
+      <c r="JS26" t="n">
         <v>24.29</v>
       </c>
     </row>
@@ -22920,7 +23154,16 @@
       <c r="JO27" s="2" t="n">
         <v>15.45</v>
       </c>
-      <c r="JP27" t="n">
+      <c r="JP27" s="2" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="JQ27" s="2" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="JR27" s="2" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="JS27" t="n">
         <v>15.45</v>
       </c>
     </row>
@@ -23752,7 +23995,16 @@
       <c r="JO28" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="JP28" t="n">
+      <c r="JP28" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="JQ28" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="JR28" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="JS28" t="n">
         <v>37</v>
       </c>
     </row>
@@ -24584,7 +24836,16 @@
       <c r="JO29" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="JP29" t="n">
+      <c r="JP29" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JQ29" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JR29" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JS29" t="n">
         <v>55</v>
       </c>
     </row>
@@ -25416,7 +25677,16 @@
       <c r="JO30" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="JP30" t="n">
+      <c r="JP30" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JQ30" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JR30" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JS30" t="n">
         <v>44</v>
       </c>
     </row>
@@ -26248,7 +26518,16 @@
       <c r="JO31" s="2" t="n">
         <v>53</v>
       </c>
-      <c r="JP31" t="n">
+      <c r="JP31" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="JQ31" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="JR31" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="JS31" t="n">
         <v>53</v>
       </c>
     </row>
@@ -27080,7 +27359,16 @@
       <c r="JO32" s="2" t="n">
         <v>2.41</v>
       </c>
-      <c r="JP32" t="n">
+      <c r="JP32" s="2" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="JQ32" s="2" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="JR32" s="2" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="JS32" t="n">
         <v>2.41</v>
       </c>
     </row>
@@ -27912,7 +28200,16 @@
       <c r="JO33" s="2" t="n">
         <v>3.79</v>
       </c>
-      <c r="JP33" t="n">
+      <c r="JP33" s="2" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="JQ33" s="2" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="JR33" s="2" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="JS33" t="n">
         <v>3.79</v>
       </c>
     </row>
@@ -28744,7 +29041,16 @@
       <c r="JO34" s="2" t="n">
         <v>39.6</v>
       </c>
-      <c r="JP34" t="n">
+      <c r="JP34" s="2" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="JQ34" s="2" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="JR34" s="2" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="JS34" t="n">
         <v>39.6</v>
       </c>
     </row>
@@ -29576,7 +29882,16 @@
       <c r="JO35" s="2" t="n">
         <v>26.4</v>
       </c>
-      <c r="JP35" t="n">
+      <c r="JP35" s="2" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="JQ35" s="2" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="JR35" s="2" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="JS35" t="n">
         <v>26.4</v>
       </c>
     </row>
@@ -30408,7 +30723,16 @@
       <c r="JO36" s="2" t="n">
         <v>187.9</v>
       </c>
-      <c r="JP36" t="n">
+      <c r="JP36" s="2" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="JQ36" s="2" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="JR36" s="2" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="JS36" t="n">
         <v>187.9</v>
       </c>
     </row>
@@ -31240,7 +31564,16 @@
       <c r="JO37" s="2" t="n">
         <v>87.3</v>
       </c>
-      <c r="JP37" t="n">
+      <c r="JP37" s="2" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="JQ37" s="2" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="JR37" s="2" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="JS37" t="n">
         <v>87.3</v>
       </c>
     </row>
@@ -32072,7 +32405,16 @@
       <c r="JO38" s="2" t="n">
         <v>25.49</v>
       </c>
-      <c r="JP38" t="n">
+      <c r="JP38" s="2" t="n">
+        <v>25.49</v>
+      </c>
+      <c r="JQ38" s="2" t="n">
+        <v>25.49</v>
+      </c>
+      <c r="JR38" s="2" t="n">
+        <v>25.49</v>
+      </c>
+      <c r="JS38" t="n">
         <v>25.49</v>
       </c>
     </row>
@@ -32904,7 +33246,16 @@
       <c r="JO39" s="2" t="n">
         <v>106.7</v>
       </c>
-      <c r="JP39" t="n">
+      <c r="JP39" s="2" t="n">
+        <v>106.7</v>
+      </c>
+      <c r="JQ39" s="2" t="n">
+        <v>106.7</v>
+      </c>
+      <c r="JR39" s="2" t="n">
+        <v>106.7</v>
+      </c>
+      <c r="JS39" t="n">
         <v>106.7</v>
       </c>
     </row>
@@ -33736,7 +34087,16 @@
       <c r="JO40" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JP40" t="n">
+      <c r="JP40" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JQ40" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JR40" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JS40" t="n">
         <v>6</v>
       </c>
     </row>
@@ -34568,7 +34928,16 @@
       <c r="JO41" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JP41" t="n">
+      <c r="JP41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JQ41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JR41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JS41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -35400,7 +35769,16 @@
       <c r="JO42" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JP42" t="n">
+      <c r="JP42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JQ42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JR42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JS42" t="n">
         <v>5</v>
       </c>
     </row>
@@ -36232,7 +36610,16 @@
       <c r="JO43" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JP43" t="n">
+      <c r="JP43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JQ43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JR43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JS43" t="n">
         <v>7</v>
       </c>
     </row>
@@ -37064,7 +37451,16 @@
       <c r="JO44" s="2" t="n">
         <v>137</v>
       </c>
-      <c r="JP44" t="n">
+      <c r="JP44" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="JQ44" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="JR44" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="JS44" t="n">
         <v>137</v>
       </c>
     </row>
@@ -37896,7 +38292,16 @@
       <c r="JO45" s="2" t="n">
         <v>194</v>
       </c>
-      <c r="JP45" t="n">
+      <c r="JP45" s="2" t="n">
+        <v>194</v>
+      </c>
+      <c r="JQ45" s="2" t="n">
+        <v>194</v>
+      </c>
+      <c r="JR45" s="2" t="n">
+        <v>194</v>
+      </c>
+      <c r="JS45" t="n">
         <v>194</v>
       </c>
     </row>
@@ -38728,7 +39133,16 @@
       <c r="JO46" s="2" t="n">
         <v>229</v>
       </c>
-      <c r="JP46" t="n">
+      <c r="JP46" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JQ46" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JR46" s="2" t="n">
+        <v>229</v>
+      </c>
+      <c r="JS46" t="n">
         <v>229</v>
       </c>
     </row>
@@ -39560,7 +39974,16 @@
       <c r="JO47" s="2" t="n">
         <v>67.40000000000001</v>
       </c>
-      <c r="JP47" t="n">
+      <c r="JP47" s="2" t="n">
+        <v>67.40000000000001</v>
+      </c>
+      <c r="JQ47" s="2" t="n">
+        <v>67.40000000000001</v>
+      </c>
+      <c r="JR47" s="2" t="n">
+        <v>67.40000000000001</v>
+      </c>
+      <c r="JS47" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -40392,7 +40815,16 @@
       <c r="JO48" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="JP48" t="n">
+      <c r="JP48" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JQ48" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JR48" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JS48" t="n">
         <v>55</v>
       </c>
     </row>
@@ -41224,7 +41656,16 @@
       <c r="JO49" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JP49" t="n">
+      <c r="JP49" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JQ49" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JR49" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JS49" t="n">
         <v>7</v>
       </c>
     </row>
@@ -42056,7 +42497,16 @@
       <c r="JO50" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="JP50" t="n">
+      <c r="JP50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JQ50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JR50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JS50" t="n">
         <v>8</v>
       </c>
     </row>
@@ -42888,7 +43338,16 @@
       <c r="JO51" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="JP51" t="n">
+      <c r="JP51" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="JQ51" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="JR51" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="JS51" t="n">
         <v>37</v>
       </c>
     </row>
@@ -43720,7 +44179,16 @@
       <c r="JO52" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="JP52" t="n">
+      <c r="JP52" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JQ52" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JR52" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JS52" t="n">
         <v>44</v>
       </c>
     </row>
@@ -44552,7 +45020,16 @@
       <c r="JO53" s="2" t="n">
         <v>70</v>
       </c>
-      <c r="JP53" t="n">
+      <c r="JP53" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="JQ53" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="JR53" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="JS53" t="n">
         <v>70</v>
       </c>
     </row>
@@ -45384,7 +45861,16 @@
       <c r="JO54" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="JP54" t="n">
+      <c r="JP54" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="JQ54" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="JR54" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="JS54" t="n">
         <v>4</v>
       </c>
     </row>
@@ -46216,7 +46702,16 @@
       <c r="JO55" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="JP55" t="n">
+      <c r="JP55" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JQ55" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JR55" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JS55" t="n">
         <v>8</v>
       </c>
     </row>
@@ -47048,7 +47543,16 @@
       <c r="JO56" s="2" t="n">
         <v>57.1</v>
       </c>
-      <c r="JP56" t="n">
+      <c r="JP56" s="2" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="JQ56" s="2" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="JR56" s="2" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="JS56" t="n">
         <v>57.1</v>
       </c>
     </row>
@@ -47880,7 +48384,16 @@
       <c r="JO57" s="2" t="n">
         <v>213</v>
       </c>
-      <c r="JP57" t="n">
+      <c r="JP57" s="2" t="n">
+        <v>213</v>
+      </c>
+      <c r="JQ57" s="2" t="n">
+        <v>213</v>
+      </c>
+      <c r="JR57" s="2" t="n">
+        <v>213</v>
+      </c>
+      <c r="JS57" t="n">
         <v>213</v>
       </c>
     </row>
@@ -48712,7 +49225,16 @@
       <c r="JO58" s="2" t="n">
         <v>103</v>
       </c>
-      <c r="JP58" t="n">
+      <c r="JP58" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="JQ58" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="JR58" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="JS58" t="n">
         <v>103</v>
       </c>
     </row>
@@ -49544,7 +50066,16 @@
       <c r="JO59" s="2" t="n">
         <v>316</v>
       </c>
-      <c r="JP59" t="n">
+      <c r="JP59" s="2" t="n">
+        <v>316</v>
+      </c>
+      <c r="JQ59" s="2" t="n">
+        <v>316</v>
+      </c>
+      <c r="JR59" s="2" t="n">
+        <v>316</v>
+      </c>
+      <c r="JS59" t="n">
         <v>316</v>
       </c>
     </row>
@@ -50376,7 +50907,16 @@
       <c r="JO60" s="2" t="n">
         <v>2.07</v>
       </c>
-      <c r="JP60" t="n">
+      <c r="JP60" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="JQ60" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="JR60" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="JS60" t="n">
         <v>2.07</v>
       </c>
     </row>
@@ -51208,7 +51748,16 @@
       <c r="JO61" s="2" t="n">
         <v>78</v>
       </c>
-      <c r="JP61" t="n">
+      <c r="JP61" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="JQ61" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="JR61" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="JS61" t="n">
         <v>78</v>
       </c>
     </row>
@@ -52040,7 +52589,16 @@
       <c r="JO62" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="JP62" t="n">
+      <c r="JP62" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="JQ62" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="JR62" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="JS62" t="n">
         <v>73</v>
       </c>
     </row>
@@ -52872,7 +53430,16 @@
       <c r="JO63" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="JP63" t="n">
+      <c r="JP63" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="JQ63" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="JR63" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="JS63" t="n">
         <v>48</v>
       </c>
     </row>
@@ -53704,7 +54271,16 @@
       <c r="JO64" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="JP64" t="n">
+      <c r="JP64" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="JQ64" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="JR64" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="JS64" t="n">
         <v>19</v>
       </c>
     </row>
@@ -54536,7 +55112,16 @@
       <c r="JO65" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="JP65" t="n">
+      <c r="JP65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JQ65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JR65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="JS65" t="n">
         <v>22</v>
       </c>
     </row>
@@ -55368,7 +55953,16 @@
       <c r="JO66" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="JP66" t="n">
+      <c r="JP66" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JQ66" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JR66" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="JS66" t="n">
         <v>11</v>
       </c>
     </row>
@@ -56200,7 +56794,16 @@
       <c r="JO67" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JP67" t="n">
+      <c r="JP67" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JQ67" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JR67" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JS67" t="n">
         <v>5</v>
       </c>
     </row>
@@ -57032,7 +57635,16 @@
       <c r="JO68" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="JP68" t="n">
+      <c r="JP68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JQ68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JR68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JS68" t="n">
         <v>10</v>
       </c>
     </row>
@@ -57864,7 +58476,16 @@
       <c r="JO69" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="JP69" t="n">
+      <c r="JP69" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JQ69" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JR69" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JS69" t="n">
         <v>3</v>
       </c>
     </row>
@@ -58696,7 +59317,16 @@
       <c r="JO70" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="JP70" t="n">
+      <c r="JP70" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="JQ70" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="JR70" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="JS70" t="n">
         <v>24</v>
       </c>
     </row>
@@ -59528,7 +60158,16 @@
       <c r="JO71" s="2" t="n">
         <v>45.8</v>
       </c>
-      <c r="JP71" t="n">
+      <c r="JP71" s="2" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="JQ71" s="2" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="JR71" s="2" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="JS71" t="n">
         <v>45.8</v>
       </c>
     </row>
@@ -60360,7 +60999,16 @@
       <c r="JO72" s="2" t="n">
         <v>28.73</v>
       </c>
-      <c r="JP72" t="n">
+      <c r="JP72" s="2" t="n">
+        <v>28.73</v>
+      </c>
+      <c r="JQ72" s="2" t="n">
+        <v>28.73</v>
+      </c>
+      <c r="JR72" s="2" t="n">
+        <v>28.73</v>
+      </c>
+      <c r="JS72" t="n">
         <v>28.73</v>
       </c>
     </row>
@@ -61192,7 +61840,16 @@
       <c r="JO73" s="2" t="n">
         <v>13.17</v>
       </c>
-      <c r="JP73" t="n">
+      <c r="JP73" s="2" t="n">
+        <v>13.17</v>
+      </c>
+      <c r="JQ73" s="2" t="n">
+        <v>13.17</v>
+      </c>
+      <c r="JR73" s="2" t="n">
+        <v>13.17</v>
+      </c>
+      <c r="JS73" t="n">
         <v>13.17</v>
       </c>
     </row>
@@ -62024,7 +62681,16 @@
       <c r="JO74" s="2" t="n">
         <v>51</v>
       </c>
-      <c r="JP74" t="n">
+      <c r="JP74" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JQ74" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JR74" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JS74" t="n">
         <v>51</v>
       </c>
     </row>
@@ -62856,7 +63522,16 @@
       <c r="JO75" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="JP75" t="n">
+      <c r="JP75" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JQ75" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JR75" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JS75" t="n">
         <v>58</v>
       </c>
     </row>
@@ -63688,7 +64363,16 @@
       <c r="JO76" s="2" t="n">
         <v>39</v>
       </c>
-      <c r="JP76" t="n">
+      <c r="JP76" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JQ76" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JR76" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JS76" t="n">
         <v>39</v>
       </c>
     </row>
@@ -64520,7 +65204,16 @@
       <c r="JO77" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="JP77" t="n">
+      <c r="JP77" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JQ77" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JR77" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JS77" t="n">
         <v>55</v>
       </c>
     </row>
@@ -65352,7 +66045,16 @@
       <c r="JO78" s="2" t="n">
         <v>2.29</v>
       </c>
-      <c r="JP78" t="n">
+      <c r="JP78" s="2" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="JQ78" s="2" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="JR78" s="2" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="JS78" t="n">
         <v>2.29</v>
       </c>
     </row>
@@ -66184,7 +66886,16 @@
       <c r="JO79" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JP79" t="n">
+      <c r="JP79" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JQ79" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JR79" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JS79" t="n">
         <v>5</v>
       </c>
     </row>
@@ -67016,7 +67727,16 @@
       <c r="JO80" s="2" t="n">
         <v>38.2</v>
       </c>
-      <c r="JP80" t="n">
+      <c r="JP80" s="2" t="n">
+        <v>38.2</v>
+      </c>
+      <c r="JQ80" s="2" t="n">
+        <v>38.2</v>
+      </c>
+      <c r="JR80" s="2" t="n">
+        <v>38.2</v>
+      </c>
+      <c r="JS80" t="n">
         <v>38.2</v>
       </c>
     </row>
@@ -67848,7 +68568,16 @@
       <c r="JO81" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="JP81" t="n">
+      <c r="JP81" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="JQ81" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="JR81" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="JS81" t="n">
         <v>20</v>
       </c>
     </row>
@@ -68680,7 +69409,16 @@
       <c r="JO82" s="2" t="n">
         <v>187.7</v>
       </c>
-      <c r="JP82" t="n">
+      <c r="JP82" s="2" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="JQ82" s="2" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="JR82" s="2" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="JS82" t="n">
         <v>187.7</v>
       </c>
     </row>
@@ -69512,7 +70250,16 @@
       <c r="JO83" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="JP83" t="n">
+      <c r="JP83" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="JQ83" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="JR83" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="JS83" t="n">
         <v>88</v>
       </c>
     </row>
@@ -70344,7 +71091,16 @@
       <c r="JO84" s="2" t="n">
         <v>26.33</v>
       </c>
-      <c r="JP84" t="n">
+      <c r="JP84" s="2" t="n">
+        <v>26.33</v>
+      </c>
+      <c r="JQ84" s="2" t="n">
+        <v>26.33</v>
+      </c>
+      <c r="JR84" s="2" t="n">
+        <v>26.33</v>
+      </c>
+      <c r="JS84" t="n">
         <v>26.33</v>
       </c>
     </row>
@@ -71176,7 +71932,16 @@
       <c r="JO85" s="2" t="n">
         <v>122.7</v>
       </c>
-      <c r="JP85" t="n">
+      <c r="JP85" s="2" t="n">
+        <v>122.7</v>
+      </c>
+      <c r="JQ85" s="2" t="n">
+        <v>122.7</v>
+      </c>
+      <c r="JR85" s="2" t="n">
+        <v>122.7</v>
+      </c>
+      <c r="JS85" t="n">
         <v>122.7</v>
       </c>
     </row>
@@ -72008,7 +72773,16 @@
       <c r="JO86" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="JP86" t="n">
+      <c r="JP86" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JQ86" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JR86" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JS86" t="n">
         <v>2</v>
       </c>
     </row>
@@ -72840,7 +73614,16 @@
       <c r="JO87" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JP87" t="n">
+      <c r="JP87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JQ87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JR87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JS87" t="n">
         <v>5</v>
       </c>
     </row>
@@ -73672,7 +74455,16 @@
       <c r="JO88" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="JP88" t="n">
+      <c r="JP88" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JQ88" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JR88" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JS88" t="n">
         <v>9</v>
       </c>
     </row>
@@ -74504,7 +75296,16 @@
       <c r="JO89" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JP89" t="n">
+      <c r="JP89" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JQ89" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JR89" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JS89" t="n">
         <v>7</v>
       </c>
     </row>
@@ -75336,7 +76137,16 @@
       <c r="JO90" s="2" t="n">
         <v>156</v>
       </c>
-      <c r="JP90" t="n">
+      <c r="JP90" s="2" t="n">
+        <v>156</v>
+      </c>
+      <c r="JQ90" s="2" t="n">
+        <v>156</v>
+      </c>
+      <c r="JR90" s="2" t="n">
+        <v>156</v>
+      </c>
+      <c r="JS90" t="n">
         <v>156</v>
       </c>
     </row>
@@ -76168,7 +76978,16 @@
       <c r="JO91" s="2" t="n">
         <v>157</v>
       </c>
-      <c r="JP91" t="n">
+      <c r="JP91" s="2" t="n">
+        <v>157</v>
+      </c>
+      <c r="JQ91" s="2" t="n">
+        <v>157</v>
+      </c>
+      <c r="JR91" s="2" t="n">
+        <v>157</v>
+      </c>
+      <c r="JS91" t="n">
         <v>157</v>
       </c>
     </row>
@@ -77000,7 +77819,16 @@
       <c r="JO92" s="2" t="n">
         <v>208</v>
       </c>
-      <c r="JP92" t="n">
+      <c r="JP92" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="JQ92" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="JR92" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="JS92" t="n">
         <v>208</v>
       </c>
     </row>
@@ -77832,7 +78660,16 @@
       <c r="JO93" s="2" t="n">
         <v>65.8</v>
       </c>
-      <c r="JP93" t="n">
+      <c r="JP93" s="2" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="JQ93" s="2" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="JR93" s="2" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="JS93" t="n">
         <v>65.8</v>
       </c>
     </row>
@@ -78664,7 +79501,16 @@
       <c r="JO94" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="JP94" t="n">
+      <c r="JP94" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JQ94" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JR94" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="JS94" t="n">
         <v>58</v>
       </c>
     </row>
@@ -79496,7 +80342,16 @@
       <c r="JO95" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="JP95" t="n">
+      <c r="JP95" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JQ95" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JR95" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="JS95" t="n">
         <v>13</v>
       </c>
     </row>
@@ -80328,7 +81183,16 @@
       <c r="JO96" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="JP96" t="n">
+      <c r="JP96" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JQ96" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JR96" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JS96" t="n">
         <v>10</v>
       </c>
     </row>
@@ -81160,7 +82024,16 @@
       <c r="JO97" s="2" t="n">
         <v>51</v>
       </c>
-      <c r="JP97" t="n">
+      <c r="JP97" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JQ97" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JR97" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JS97" t="n">
         <v>51</v>
       </c>
     </row>
@@ -81992,7 +82865,16 @@
       <c r="JO98" s="2" t="n">
         <v>39</v>
       </c>
-      <c r="JP98" t="n">
+      <c r="JP98" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JQ98" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JR98" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JS98" t="n">
         <v>39</v>
       </c>
     </row>
@@ -82824,7 +83706,16 @@
       <c r="JO99" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="JP99" t="n">
+      <c r="JP99" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JQ99" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JR99" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JS99" t="n">
         <v>44</v>
       </c>
     </row>
@@ -83656,7 +84547,16 @@
       <c r="JO100" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="JP100" t="n">
+      <c r="JP100" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JQ100" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JR100" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JS100" t="n">
         <v>3</v>
       </c>
     </row>
@@ -84488,7 +85388,16 @@
       <c r="JO101" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JP101" t="n">
+      <c r="JP101" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JQ101" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JR101" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JS101" t="n">
         <v>5</v>
       </c>
     </row>
@@ -85320,7 +86229,16 @@
       <c r="JO102" s="2" t="n">
         <v>45.5</v>
       </c>
-      <c r="JP102" t="n">
+      <c r="JP102" s="2" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="JQ102" s="2" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="JR102" s="2" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="JS102" t="n">
         <v>45.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added error check to ensure rounds that have had data gathered cannot be further updated once upcoming predictions have been generated. This would give wrong team PAVs and venues etc. as dataframe shapes would be misaligned.
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Brisbane_stats.xlsx
+++ b/django_AFL_ML/Data/Brisbane_stats.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:KP102"/>
+  <dimension ref="A1:KU102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="HZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="IL36" activeCellId="0" sqref="IL36"/>
@@ -1366,7 +1366,22 @@
       <c r="KO1" s="2" t="n">
         <v>10748</v>
       </c>
-      <c r="KP1" t="n">
+      <c r="KP1" s="2" t="n">
+        <v>10748</v>
+      </c>
+      <c r="KQ1" s="2" t="n">
+        <v>10748</v>
+      </c>
+      <c r="KR1" s="2" t="n">
+        <v>10748</v>
+      </c>
+      <c r="KS1" s="2" t="n">
+        <v>10748</v>
+      </c>
+      <c r="KT1" s="2" t="n">
+        <v>10748</v>
+      </c>
+      <c r="KU1" t="n">
         <v>10748</v>
       </c>
     </row>
@@ -2276,7 +2291,22 @@
       <c r="KO2" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="KP2" t="n">
+      <c r="KP2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="KQ2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="KR2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="KS2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="KT2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="KU2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -3186,7 +3216,22 @@
       <c r="KO3" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="KP3" t="n">
+      <c r="KP3" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="KQ3" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="KR3" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="KS3" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="KT3" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="KU3" t="n">
         <v>27</v>
       </c>
     </row>
@@ -4096,7 +4141,22 @@
       <c r="KO4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="KP4" t="n">
+      <c r="KP4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KQ4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KR4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KS4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KT4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KU4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5006,7 +5066,22 @@
       <c r="KO5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="KP5" t="n">
+      <c r="KP5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KQ5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KR5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KS5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KT5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KU5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5916,7 +5991,22 @@
       <c r="KO6" s="2" t="n">
         <v>49</v>
       </c>
-      <c r="KP6" t="n">
+      <c r="KP6" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="KQ6" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="KR6" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="KS6" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="KT6" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="KU6" t="n">
         <v>49</v>
       </c>
     </row>
@@ -6826,7 +6916,22 @@
       <c r="KO7" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="KP7" t="n">
+      <c r="KP7" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="KQ7" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="KR7" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="KS7" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="KT7" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="KU7" t="n">
         <v>120</v>
       </c>
     </row>
@@ -7736,7 +7841,22 @@
       <c r="KO8" s="2" t="n">
         <v>-71</v>
       </c>
-      <c r="KP8" t="n">
+      <c r="KP8" s="2" t="n">
+        <v>-71</v>
+      </c>
+      <c r="KQ8" s="2" t="n">
+        <v>-71</v>
+      </c>
+      <c r="KR8" s="2" t="n">
+        <v>-71</v>
+      </c>
+      <c r="KS8" s="2" t="n">
+        <v>-71</v>
+      </c>
+      <c r="KT8" s="2" t="n">
+        <v>-71</v>
+      </c>
+      <c r="KU8" t="n">
         <v>-71</v>
       </c>
     </row>
@@ -8646,7 +8766,22 @@
       <c r="KO9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="KP9" t="n">
+      <c r="KP9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KQ9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KR9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KS9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KT9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KU9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9556,7 +9691,22 @@
       <c r="KO10" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KP10" t="n">
+      <c r="KP10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KQ10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KR10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KS10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KT10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KU10" t="n">
         <v>7</v>
       </c>
     </row>
@@ -10466,7 +10616,22 @@
       <c r="KO11" s="2" t="n">
         <v>197</v>
       </c>
-      <c r="KP11" t="n">
+      <c r="KP11" s="2" t="n">
+        <v>197</v>
+      </c>
+      <c r="KQ11" s="2" t="n">
+        <v>197</v>
+      </c>
+      <c r="KR11" s="2" t="n">
+        <v>197</v>
+      </c>
+      <c r="KS11" s="2" t="n">
+        <v>197</v>
+      </c>
+      <c r="KT11" s="2" t="n">
+        <v>197</v>
+      </c>
+      <c r="KU11" t="n">
         <v>197</v>
       </c>
     </row>
@@ -11376,7 +11541,22 @@
       <c r="KO12" s="2" t="n">
         <v>99</v>
       </c>
-      <c r="KP12" t="n">
+      <c r="KP12" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="KQ12" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="KR12" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="KS12" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="KT12" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="KU12" t="n">
         <v>99</v>
       </c>
     </row>
@@ -12286,7 +12466,22 @@
       <c r="KO13" s="2" t="n">
         <v>296</v>
       </c>
-      <c r="KP13" t="n">
+      <c r="KP13" s="2" t="n">
+        <v>296</v>
+      </c>
+      <c r="KQ13" s="2" t="n">
+        <v>296</v>
+      </c>
+      <c r="KR13" s="2" t="n">
+        <v>296</v>
+      </c>
+      <c r="KS13" s="2" t="n">
+        <v>296</v>
+      </c>
+      <c r="KT13" s="2" t="n">
+        <v>296</v>
+      </c>
+      <c r="KU13" t="n">
         <v>296</v>
       </c>
     </row>
@@ -13196,7 +13391,22 @@
       <c r="KO14" s="2" t="n">
         <v>1.99</v>
       </c>
-      <c r="KP14" t="n">
+      <c r="KP14" s="2" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="KQ14" s="2" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="KR14" s="2" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="KS14" s="2" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="KT14" s="2" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="KU14" t="n">
         <v>1.99</v>
       </c>
     </row>
@@ -14106,7 +14316,22 @@
       <c r="KO15" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="KP15" t="n">
+      <c r="KP15" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="KQ15" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="KR15" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="KS15" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="KT15" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="KU15" t="n">
         <v>88</v>
       </c>
     </row>
@@ -15016,7 +15241,22 @@
       <c r="KO16" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="KP16" t="n">
+      <c r="KP16" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="KQ16" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="KR16" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="KS16" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="KT16" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="KU16" t="n">
         <v>68</v>
       </c>
     </row>
@@ -15926,7 +16166,22 @@
       <c r="KO17" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KP17" t="n">
+      <c r="KP17" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KQ17" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KR17" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KS17" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KT17" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KU17" t="n">
         <v>41</v>
       </c>
     </row>
@@ -16836,7 +17091,22 @@
       <c r="KO18" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="KP18" t="n">
+      <c r="KP18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="KQ18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="KR18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="KS18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="KT18" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="KU18" t="n">
         <v>22</v>
       </c>
     </row>
@@ -17746,7 +18016,22 @@
       <c r="KO19" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KP19" t="n">
+      <c r="KP19" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KQ19" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KR19" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KS19" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KT19" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KU19" t="n">
         <v>13</v>
       </c>
     </row>
@@ -18656,7 +18941,22 @@
       <c r="KO20" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KP20" t="n">
+      <c r="KP20" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KQ20" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KR20" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KS20" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KT20" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KU20" t="n">
         <v>7</v>
       </c>
     </row>
@@ -19566,7 +19866,22 @@
       <c r="KO21" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KP21" t="n">
+      <c r="KP21" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KQ21" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KR21" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KS21" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KT21" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KU21" t="n">
         <v>7</v>
       </c>
     </row>
@@ -20476,7 +20791,22 @@
       <c r="KO22" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KP22" t="n">
+      <c r="KP22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KQ22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KR22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KS22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KT22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KU22" t="n">
         <v>7</v>
       </c>
     </row>
@@ -21386,7 +21716,22 @@
       <c r="KO23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="KP23" t="n">
+      <c r="KP23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KQ23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KR23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KS23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KT23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KU23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -22296,7 +22641,22 @@
       <c r="KO24" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="KP24" t="n">
+      <c r="KP24" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KQ24" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KR24" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KS24" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KT24" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KU24" t="n">
         <v>14</v>
       </c>
     </row>
@@ -23206,7 +23566,22 @@
       <c r="KO25" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KP25" t="n">
+      <c r="KP25" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KQ25" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KR25" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KS25" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KT25" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KU25" t="n">
         <v>50</v>
       </c>
     </row>
@@ -24116,7 +24491,22 @@
       <c r="KO26" s="2" t="n">
         <v>42.29</v>
       </c>
-      <c r="KP26" t="n">
+      <c r="KP26" s="2" t="n">
+        <v>42.29</v>
+      </c>
+      <c r="KQ26" s="2" t="n">
+        <v>42.29</v>
+      </c>
+      <c r="KR26" s="2" t="n">
+        <v>42.29</v>
+      </c>
+      <c r="KS26" s="2" t="n">
+        <v>42.29</v>
+      </c>
+      <c r="KT26" s="2" t="n">
+        <v>42.29</v>
+      </c>
+      <c r="KU26" t="n">
         <v>42.29</v>
       </c>
     </row>
@@ -25026,7 +25416,22 @@
       <c r="KO27" s="2" t="n">
         <v>21.14</v>
       </c>
-      <c r="KP27" t="n">
+      <c r="KP27" s="2" t="n">
+        <v>21.14</v>
+      </c>
+      <c r="KQ27" s="2" t="n">
+        <v>21.14</v>
+      </c>
+      <c r="KR27" s="2" t="n">
+        <v>21.14</v>
+      </c>
+      <c r="KS27" s="2" t="n">
+        <v>21.14</v>
+      </c>
+      <c r="KT27" s="2" t="n">
+        <v>21.14</v>
+      </c>
+      <c r="KU27" t="n">
         <v>21.14</v>
       </c>
     </row>
@@ -25936,7 +26341,22 @@
       <c r="KO28" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="KP28" t="n">
+      <c r="KP28" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KQ28" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KR28" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KS28" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KT28" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KU28" t="n">
         <v>40</v>
       </c>
     </row>
@@ -26846,7 +27266,22 @@
       <c r="KO29" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KP29" t="n">
+      <c r="KP29" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KQ29" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KR29" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KS29" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KT29" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KU29" t="n">
         <v>50</v>
       </c>
     </row>
@@ -27756,7 +28191,22 @@
       <c r="KO30" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KP30" t="n">
+      <c r="KP30" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KQ30" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KR30" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KS30" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KT30" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KU30" t="n">
         <v>41</v>
       </c>
     </row>
@@ -28666,7 +29116,22 @@
       <c r="KO31" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="KP31" t="n">
+      <c r="KP31" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="KQ31" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="KR31" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="KS31" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="KT31" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="KU31" t="n">
         <v>46</v>
       </c>
     </row>
@@ -29576,7 +30041,22 @@
       <c r="KO32" s="2" t="n">
         <v>3.29</v>
       </c>
-      <c r="KP32" t="n">
+      <c r="KP32" s="2" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="KQ32" s="2" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="KR32" s="2" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="KS32" s="2" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="KT32" s="2" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="KU32" t="n">
         <v>3.29</v>
       </c>
     </row>
@@ -30486,7 +30966,22 @@
       <c r="KO33" s="2" t="n">
         <v>6.57</v>
       </c>
-      <c r="KP33" t="n">
+      <c r="KP33" s="2" t="n">
+        <v>6.57</v>
+      </c>
+      <c r="KQ33" s="2" t="n">
+        <v>6.57</v>
+      </c>
+      <c r="KR33" s="2" t="n">
+        <v>6.57</v>
+      </c>
+      <c r="KS33" s="2" t="n">
+        <v>6.57</v>
+      </c>
+      <c r="KT33" s="2" t="n">
+        <v>6.57</v>
+      </c>
+      <c r="KU33" t="n">
         <v>6.57</v>
       </c>
     </row>
@@ -31396,7 +31891,22 @@
       <c r="KO34" s="2" t="n">
         <v>30.4</v>
       </c>
-      <c r="KP34" t="n">
+      <c r="KP34" s="2" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="KQ34" s="2" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="KR34" s="2" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="KS34" s="2" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="KT34" s="2" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="KU34" t="n">
         <v>30.4</v>
       </c>
     </row>
@@ -32306,7 +32816,22 @@
       <c r="KO35" s="2" t="n">
         <v>15.2</v>
       </c>
-      <c r="KP35" t="n">
+      <c r="KP35" s="2" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="KQ35" s="2" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="KR35" s="2" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="KS35" s="2" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="KT35" s="2" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="KU35" t="n">
         <v>15.2</v>
       </c>
     </row>
@@ -33216,7 +33741,22 @@
       <c r="KO36" s="2" t="n">
         <v>187.9</v>
       </c>
-      <c r="KP36" t="n">
+      <c r="KP36" s="2" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="KQ36" s="2" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="KR36" s="2" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="KS36" s="2" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="KT36" s="2" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="KU36" t="n">
         <v>187.9</v>
       </c>
     </row>
@@ -34126,7 +34666,22 @@
       <c r="KO37" s="2" t="n">
         <v>87.8</v>
       </c>
-      <c r="KP37" t="n">
+      <c r="KP37" s="2" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="KQ37" s="2" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="KR37" s="2" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="KS37" s="2" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="KT37" s="2" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="KU37" t="n">
         <v>87.8</v>
       </c>
     </row>
@@ -35036,7 +35591,22 @@
       <c r="KO38" s="2" t="n">
         <v>25.66</v>
       </c>
-      <c r="KP38" t="n">
+      <c r="KP38" s="2" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="KQ38" s="2" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="KR38" s="2" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="KS38" s="2" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="KT38" s="2" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="KU38" t="n">
         <v>25.66</v>
       </c>
     </row>
@@ -35946,7 +36516,22 @@
       <c r="KO39" s="2" t="n">
         <v>116.6</v>
       </c>
-      <c r="KP39" t="n">
+      <c r="KP39" s="2" t="n">
+        <v>116.6</v>
+      </c>
+      <c r="KQ39" s="2" t="n">
+        <v>116.6</v>
+      </c>
+      <c r="KR39" s="2" t="n">
+        <v>116.6</v>
+      </c>
+      <c r="KS39" s="2" t="n">
+        <v>116.6</v>
+      </c>
+      <c r="KT39" s="2" t="n">
+        <v>116.6</v>
+      </c>
+      <c r="KU39" t="n">
         <v>116.6</v>
       </c>
     </row>
@@ -36856,7 +37441,22 @@
       <c r="KO40" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="KP40" t="n">
+      <c r="KP40" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="KQ40" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="KR40" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="KS40" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="KT40" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="KU40" t="n">
         <v>4</v>
       </c>
     </row>
@@ -37766,7 +38366,22 @@
       <c r="KO41" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="KP41" t="n">
+      <c r="KP41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KQ41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KR41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KS41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KT41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KU41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -38676,7 +39291,22 @@
       <c r="KO42" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="KP42" t="n">
+      <c r="KP42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KQ42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KR42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KS42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KT42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KU42" t="n">
         <v>6</v>
       </c>
     </row>
@@ -39586,7 +40216,22 @@
       <c r="KO43" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KP43" t="n">
+      <c r="KP43" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KQ43" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KR43" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KS43" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KT43" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KU43" t="n">
         <v>8</v>
       </c>
     </row>
@@ -40496,7 +41141,22 @@
       <c r="KO44" s="2" t="n">
         <v>117</v>
       </c>
-      <c r="KP44" t="n">
+      <c r="KP44" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="KQ44" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="KR44" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="KS44" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="KT44" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="KU44" t="n">
         <v>117</v>
       </c>
     </row>
@@ -41406,7 +42066,22 @@
       <c r="KO45" s="2" t="n">
         <v>177</v>
       </c>
-      <c r="KP45" t="n">
+      <c r="KP45" s="2" t="n">
+        <v>177</v>
+      </c>
+      <c r="KQ45" s="2" t="n">
+        <v>177</v>
+      </c>
+      <c r="KR45" s="2" t="n">
+        <v>177</v>
+      </c>
+      <c r="KS45" s="2" t="n">
+        <v>177</v>
+      </c>
+      <c r="KT45" s="2" t="n">
+        <v>177</v>
+      </c>
+      <c r="KU45" t="n">
         <v>177</v>
       </c>
     </row>
@@ -42316,7 +42991,22 @@
       <c r="KO46" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="KP46" t="n">
+      <c r="KP46" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="KQ46" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="KR46" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="KS46" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="KT46" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="KU46" t="n">
         <v>200</v>
       </c>
     </row>
@@ -43226,7 +43916,22 @@
       <c r="KO47" s="2" t="n">
         <v>67.59999999999999</v>
       </c>
-      <c r="KP47" t="n">
+      <c r="KP47" s="2" t="n">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="KQ47" s="2" t="n">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="KR47" s="2" t="n">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="KS47" s="2" t="n">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="KT47" s="2" t="n">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="KU47" t="n">
         <v>67.59999999999999</v>
       </c>
     </row>
@@ -44136,7 +44841,22 @@
       <c r="KO48" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KP48" t="n">
+      <c r="KP48" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KQ48" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KR48" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KS48" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KT48" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="KU48" t="n">
         <v>50</v>
       </c>
     </row>
@@ -45046,7 +45766,22 @@
       <c r="KO49" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KP49" t="n">
+      <c r="KP49" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KQ49" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KR49" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KS49" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KT49" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KU49" t="n">
         <v>8</v>
       </c>
     </row>
@@ -45956,7 +46691,22 @@
       <c r="KO50" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="KP50" t="n">
+      <c r="KP50" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="KQ50" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="KR50" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="KS50" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="KT50" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="KU50" t="n">
         <v>11</v>
       </c>
     </row>
@@ -46866,7 +47616,22 @@
       <c r="KO51" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="KP51" t="n">
+      <c r="KP51" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KQ51" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KR51" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KS51" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KT51" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="KU51" t="n">
         <v>40</v>
       </c>
     </row>
@@ -47776,7 +48541,22 @@
       <c r="KO52" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KP52" t="n">
+      <c r="KP52" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KQ52" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KR52" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KS52" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KT52" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KU52" t="n">
         <v>41</v>
       </c>
     </row>
@@ -48686,7 +49466,22 @@
       <c r="KO53" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KP53" t="n">
+      <c r="KP53" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KQ53" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KR53" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KS53" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KT53" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KU53" t="n">
         <v>37</v>
       </c>
     </row>
@@ -49596,7 +50391,22 @@
       <c r="KO54" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="KP54" t="n">
+      <c r="KP54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KQ54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KR54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KS54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KT54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KU54" t="n">
         <v>1</v>
       </c>
     </row>
@@ -50506,7 +51316,22 @@
       <c r="KO55" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KP55" t="n">
+      <c r="KP55" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KQ55" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KR55" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KS55" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KT55" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="KU55" t="n">
         <v>7</v>
       </c>
     </row>
@@ -51416,7 +52241,22 @@
       <c r="KO56" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="KP56" t="n">
+      <c r="KP56" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="KQ56" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="KR56" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="KS56" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="KT56" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="KU56" t="n">
         <v>100</v>
       </c>
     </row>
@@ -52326,7 +53166,22 @@
       <c r="KO57" s="2" t="n">
         <v>209</v>
       </c>
-      <c r="KP57" t="n">
+      <c r="KP57" s="2" t="n">
+        <v>209</v>
+      </c>
+      <c r="KQ57" s="2" t="n">
+        <v>209</v>
+      </c>
+      <c r="KR57" s="2" t="n">
+        <v>209</v>
+      </c>
+      <c r="KS57" s="2" t="n">
+        <v>209</v>
+      </c>
+      <c r="KT57" s="2" t="n">
+        <v>209</v>
+      </c>
+      <c r="KU57" t="n">
         <v>209</v>
       </c>
     </row>
@@ -53236,7 +54091,22 @@
       <c r="KO58" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="KP58" t="n">
+      <c r="KP58" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="KQ58" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="KR58" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="KS58" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="KT58" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="KU58" t="n">
         <v>152</v>
       </c>
     </row>
@@ -54146,7 +55016,22 @@
       <c r="KO59" s="2" t="n">
         <v>361</v>
       </c>
-      <c r="KP59" t="n">
+      <c r="KP59" s="2" t="n">
+        <v>361</v>
+      </c>
+      <c r="KQ59" s="2" t="n">
+        <v>361</v>
+      </c>
+      <c r="KR59" s="2" t="n">
+        <v>361</v>
+      </c>
+      <c r="KS59" s="2" t="n">
+        <v>361</v>
+      </c>
+      <c r="KT59" s="2" t="n">
+        <v>361</v>
+      </c>
+      <c r="KU59" t="n">
         <v>361</v>
       </c>
     </row>
@@ -55056,7 +55941,22 @@
       <c r="KO60" s="2" t="n">
         <v>1.38</v>
       </c>
-      <c r="KP60" t="n">
+      <c r="KP60" s="2" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="KQ60" s="2" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="KR60" s="2" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="KS60" s="2" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="KT60" s="2" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="KU60" t="n">
         <v>1.38</v>
       </c>
     </row>
@@ -55966,7 +56866,22 @@
       <c r="KO61" s="2" t="n">
         <v>102</v>
       </c>
-      <c r="KP61" t="n">
+      <c r="KP61" s="2" t="n">
+        <v>102</v>
+      </c>
+      <c r="KQ61" s="2" t="n">
+        <v>102</v>
+      </c>
+      <c r="KR61" s="2" t="n">
+        <v>102</v>
+      </c>
+      <c r="KS61" s="2" t="n">
+        <v>102</v>
+      </c>
+      <c r="KT61" s="2" t="n">
+        <v>102</v>
+      </c>
+      <c r="KU61" t="n">
         <v>102</v>
       </c>
     </row>
@@ -56876,7 +57791,22 @@
       <c r="KO62" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="KP62" t="n">
+      <c r="KP62" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="KQ62" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="KR62" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="KS62" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="KT62" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="KU62" t="n">
         <v>65</v>
       </c>
     </row>
@@ -57786,7 +58716,22 @@
       <c r="KO63" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KP63" t="n">
+      <c r="KP63" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KQ63" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KR63" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KS63" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KT63" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="KU63" t="n">
         <v>41</v>
       </c>
     </row>
@@ -58696,7 +59641,22 @@
       <c r="KO64" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KP64" t="n">
+      <c r="KP64" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KQ64" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KR64" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KS64" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KT64" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KU64" t="n">
         <v>13</v>
       </c>
     </row>
@@ -59606,7 +60566,22 @@
       <c r="KO65" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="KP65" t="n">
+      <c r="KP65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="KQ65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="KR65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="KS65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="KT65" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="KU65" t="n">
         <v>22</v>
       </c>
     </row>
@@ -60516,7 +61491,22 @@
       <c r="KO66" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="KP66" t="n">
+      <c r="KP66" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="KQ66" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="KR66" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="KS66" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="KT66" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="KU66" t="n">
         <v>18</v>
       </c>
     </row>
@@ -61426,7 +62416,22 @@
       <c r="KO67" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="KP67" t="n">
+      <c r="KP67" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KQ67" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KR67" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KS67" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KT67" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KU67" t="n">
         <v>14</v>
       </c>
     </row>
@@ -62336,7 +63341,22 @@
       <c r="KO68" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="KP68" t="n">
+      <c r="KP68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="KQ68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="KR68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="KS68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="KT68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="KU68" t="n">
         <v>10</v>
       </c>
     </row>
@@ -63246,7 +64266,22 @@
       <c r="KO69" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="KP69" t="n">
+      <c r="KP69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="KQ69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="KR69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="KS69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="KT69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="KU69" t="n">
         <v>2</v>
       </c>
     </row>
@@ -64156,7 +65191,22 @@
       <c r="KO70" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="KP70" t="n">
+      <c r="KP70" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="KQ70" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="KR70" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="KS70" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="KT70" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="KU70" t="n">
         <v>30</v>
       </c>
     </row>
@@ -65066,7 +66116,22 @@
       <c r="KO71" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="KP71" t="n">
+      <c r="KP71" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="KQ71" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="KR71" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="KS71" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="KT71" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="KU71" t="n">
         <v>60</v>
       </c>
     </row>
@@ -65976,7 +67041,22 @@
       <c r="KO72" s="2" t="n">
         <v>20.06</v>
       </c>
-      <c r="KP72" t="n">
+      <c r="KP72" s="2" t="n">
+        <v>20.06</v>
+      </c>
+      <c r="KQ72" s="2" t="n">
+        <v>20.06</v>
+      </c>
+      <c r="KR72" s="2" t="n">
+        <v>20.06</v>
+      </c>
+      <c r="KS72" s="2" t="n">
+        <v>20.06</v>
+      </c>
+      <c r="KT72" s="2" t="n">
+        <v>20.06</v>
+      </c>
+      <c r="KU72" t="n">
         <v>20.06</v>
       </c>
     </row>
@@ -66886,7 +67966,22 @@
       <c r="KO73" s="2" t="n">
         <v>12.03</v>
       </c>
-      <c r="KP73" t="n">
+      <c r="KP73" s="2" t="n">
+        <v>12.03</v>
+      </c>
+      <c r="KQ73" s="2" t="n">
+        <v>12.03</v>
+      </c>
+      <c r="KR73" s="2" t="n">
+        <v>12.03</v>
+      </c>
+      <c r="KS73" s="2" t="n">
+        <v>12.03</v>
+      </c>
+      <c r="KT73" s="2" t="n">
+        <v>12.03</v>
+      </c>
+      <c r="KU73" t="n">
         <v>12.03</v>
       </c>
     </row>
@@ -67796,7 +68891,22 @@
       <c r="KO74" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KP74" t="n">
+      <c r="KP74" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KQ74" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KR74" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KS74" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KT74" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KU74" t="n">
         <v>37</v>
       </c>
     </row>
@@ -68706,7 +69816,22 @@
       <c r="KO75" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="KP75" t="n">
+      <c r="KP75" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KQ75" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KR75" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KS75" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KT75" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KU75" t="n">
         <v>55</v>
       </c>
     </row>
@@ -69616,7 +70741,22 @@
       <c r="KO76" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="KP76" t="n">
+      <c r="KP76" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KQ76" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KR76" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KS76" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KT76" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KU76" t="n">
         <v>38</v>
       </c>
     </row>
@@ -70526,7 +71666,22 @@
       <c r="KO77" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="KP77" t="n">
+      <c r="KP77" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="KQ77" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="KR77" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="KS77" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="KT77" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="KU77" t="n">
         <v>59</v>
       </c>
     </row>
@@ -71436,7 +72591,22 @@
       <c r="KO78" s="2" t="n">
         <v>1.97</v>
       </c>
-      <c r="KP78" t="n">
+      <c r="KP78" s="2" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="KQ78" s="2" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="KR78" s="2" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="KS78" s="2" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="KT78" s="2" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="KU78" t="n">
         <v>1.97</v>
       </c>
     </row>
@@ -72346,7 +73516,22 @@
       <c r="KO79" s="2" t="n">
         <v>3.28</v>
       </c>
-      <c r="KP79" t="n">
+      <c r="KP79" s="2" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="KQ79" s="2" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="KR79" s="2" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="KS79" s="2" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="KT79" s="2" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="KU79" t="n">
         <v>3.28</v>
       </c>
     </row>
@@ -73256,7 +74441,22 @@
       <c r="KO80" s="2" t="n">
         <v>47.5</v>
       </c>
-      <c r="KP80" t="n">
+      <c r="KP80" s="2" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="KQ80" s="2" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="KR80" s="2" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="KS80" s="2" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="KT80" s="2" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="KU80" t="n">
         <v>47.5</v>
       </c>
     </row>
@@ -74166,7 +75366,22 @@
       <c r="KO81" s="2" t="n">
         <v>30.5</v>
       </c>
-      <c r="KP81" t="n">
+      <c r="KP81" s="2" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="KQ81" s="2" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="KR81" s="2" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="KS81" s="2" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="KT81" s="2" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="KU81" t="n">
         <v>30.5</v>
       </c>
     </row>
@@ -75076,7 +76291,22 @@
       <c r="KO82" s="2" t="n">
         <v>188.9</v>
       </c>
-      <c r="KP82" t="n">
+      <c r="KP82" s="2" t="n">
+        <v>188.9</v>
+      </c>
+      <c r="KQ82" s="2" t="n">
+        <v>188.9</v>
+      </c>
+      <c r="KR82" s="2" t="n">
+        <v>188.9</v>
+      </c>
+      <c r="KS82" s="2" t="n">
+        <v>188.9</v>
+      </c>
+      <c r="KT82" s="2" t="n">
+        <v>188.9</v>
+      </c>
+      <c r="KU82" t="n">
         <v>188.9</v>
       </c>
     </row>
@@ -75986,7 +77216,22 @@
       <c r="KO83" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="KP83" t="n">
+      <c r="KP83" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="KQ83" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="KR83" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="KS83" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="KT83" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="KU83" t="n">
         <v>88</v>
       </c>
     </row>
@@ -76896,7 +78141,22 @@
       <c r="KO84" s="2" t="n">
         <v>28.33</v>
       </c>
-      <c r="KP84" t="n">
+      <c r="KP84" s="2" t="n">
+        <v>28.33</v>
+      </c>
+      <c r="KQ84" s="2" t="n">
+        <v>28.33</v>
+      </c>
+      <c r="KR84" s="2" t="n">
+        <v>28.33</v>
+      </c>
+      <c r="KS84" s="2" t="n">
+        <v>28.33</v>
+      </c>
+      <c r="KT84" s="2" t="n">
+        <v>28.33</v>
+      </c>
+      <c r="KU84" t="n">
         <v>28.33</v>
       </c>
     </row>
@@ -77806,7 +79066,22 @@
       <c r="KO85" s="2" t="n">
         <v>163.1</v>
       </c>
-      <c r="KP85" t="n">
+      <c r="KP85" s="2" t="n">
+        <v>163.1</v>
+      </c>
+      <c r="KQ85" s="2" t="n">
+        <v>163.1</v>
+      </c>
+      <c r="KR85" s="2" t="n">
+        <v>163.1</v>
+      </c>
+      <c r="KS85" s="2" t="n">
+        <v>163.1</v>
+      </c>
+      <c r="KT85" s="2" t="n">
+        <v>163.1</v>
+      </c>
+      <c r="KU85" t="n">
         <v>163.1</v>
       </c>
     </row>
@@ -78716,7 +79991,22 @@
       <c r="KO86" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="KP86" t="n">
+      <c r="KP86" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="KQ86" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="KR86" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="KS86" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="KT86" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="KU86" t="n">
         <v>3</v>
       </c>
     </row>
@@ -79626,7 +80916,22 @@
       <c r="KO87" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="KP87" t="n">
+      <c r="KP87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KQ87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KR87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KS87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KT87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="KU87" t="n">
         <v>5</v>
       </c>
     </row>
@@ -80536,7 +81841,22 @@
       <c r="KO88" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="KP88" t="n">
+      <c r="KP88" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="KQ88" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="KR88" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="KS88" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="KT88" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="KU88" t="n">
         <v>2</v>
       </c>
     </row>
@@ -81446,7 +82766,22 @@
       <c r="KO89" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KP89" t="n">
+      <c r="KP89" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KQ89" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KR89" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KS89" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KT89" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="KU89" t="n">
         <v>13</v>
       </c>
     </row>
@@ -82356,7 +83691,22 @@
       <c r="KO90" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="KP90" t="n">
+      <c r="KP90" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="KQ90" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="KR90" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="KS90" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="KT90" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="KU90" t="n">
         <v>125</v>
       </c>
     </row>
@@ -83266,7 +84616,22 @@
       <c r="KO91" s="2" t="n">
         <v>230</v>
       </c>
-      <c r="KP91" t="n">
+      <c r="KP91" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="KQ91" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="KR91" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="KS91" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="KT91" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="KU91" t="n">
         <v>230</v>
       </c>
     </row>
@@ -84176,7 +85541,22 @@
       <c r="KO92" s="2" t="n">
         <v>274</v>
       </c>
-      <c r="KP92" t="n">
+      <c r="KP92" s="2" t="n">
+        <v>274</v>
+      </c>
+      <c r="KQ92" s="2" t="n">
+        <v>274</v>
+      </c>
+      <c r="KR92" s="2" t="n">
+        <v>274</v>
+      </c>
+      <c r="KS92" s="2" t="n">
+        <v>274</v>
+      </c>
+      <c r="KT92" s="2" t="n">
+        <v>274</v>
+      </c>
+      <c r="KU92" t="n">
         <v>274</v>
       </c>
     </row>
@@ -85086,7 +86466,22 @@
       <c r="KO93" s="2" t="n">
         <v>75.90000000000001</v>
       </c>
-      <c r="KP93" t="n">
+      <c r="KP93" s="2" t="n">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="KQ93" s="2" t="n">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="KR93" s="2" t="n">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="KS93" s="2" t="n">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="KT93" s="2" t="n">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="KU93" t="n">
         <v>75.90000000000001</v>
       </c>
     </row>
@@ -85996,7 +87391,22 @@
       <c r="KO94" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="KP94" t="n">
+      <c r="KP94" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KQ94" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KR94" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KS94" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KT94" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="KU94" t="n">
         <v>55</v>
       </c>
     </row>
@@ -86906,7 +88316,22 @@
       <c r="KO95" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="KP95" t="n">
+      <c r="KP95" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="KQ95" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="KR95" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="KS95" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="KT95" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="KU95" t="n">
         <v>15</v>
       </c>
     </row>
@@ -87816,7 +89241,22 @@
       <c r="KO96" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="KP96" t="n">
+      <c r="KP96" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="KQ96" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="KR96" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="KS96" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="KT96" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="KU96" t="n">
         <v>15</v>
       </c>
     </row>
@@ -88726,7 +90166,22 @@
       <c r="KO97" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KP97" t="n">
+      <c r="KP97" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KQ97" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KR97" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KS97" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KT97" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="KU97" t="n">
         <v>37</v>
       </c>
     </row>
@@ -89636,7 +91091,22 @@
       <c r="KO98" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="KP98" t="n">
+      <c r="KP98" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KQ98" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KR98" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KS98" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KT98" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="KU98" t="n">
         <v>38</v>
       </c>
     </row>
@@ -90546,7 +92016,22 @@
       <c r="KO99" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="KP99" t="n">
+      <c r="KP99" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="KQ99" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="KR99" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="KS99" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="KT99" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="KU99" t="n">
         <v>48</v>
       </c>
     </row>
@@ -91456,7 +92941,22 @@
       <c r="KO100" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KP100" t="n">
+      <c r="KP100" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KQ100" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KR100" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KS100" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KT100" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="KU100" t="n">
         <v>8</v>
       </c>
     </row>
@@ -92366,7 +93866,22 @@
       <c r="KO101" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="KP101" t="n">
+      <c r="KP101" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KQ101" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KR101" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KS101" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KT101" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="KU101" t="n">
         <v>14</v>
       </c>
     </row>
@@ -93276,7 +94791,22 @@
       <c r="KO102" s="2" t="n">
         <v>77.8</v>
       </c>
-      <c r="KP102" t="n">
+      <c r="KP102" s="2" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="KQ102" s="2" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="KR102" s="2" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="KS102" s="2" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="KT102" s="2" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="KU102" t="n">
         <v>77.8</v>
       </c>
     </row>

</xml_diff>